<commit_message>
add more jdt cases
</commit_message>
<xml_diff>
--- a/jdt-plus5.xlsx
+++ b/jdt-plus5.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>issueID</t>
   </si>
@@ -98,10 +98,73 @@
     <t>Upsilon</t>
   </si>
   <si>
+    <t>ProblemReasons-&gt;IProblem-&gt;ProblemReporter-&gt;ModuleDeclaration</t>
+  </si>
+  <si>
+    <t>Visitor pattern; change visitor and classes A which call, typed visitor; and one class use one of A</t>
+  </si>
+  <si>
+    <t>Lambda, Domino</t>
+  </si>
+  <si>
+    <t>AssistParser-&gt;CompletionParser-&gt;UnresolvedReferenceNameFinder-&gt;CompletionEngine; RelevanceConstants-&gt;CompletionEngine</t>
+  </si>
+  <si>
+    <t>ProblemReasons adds a field. Scope, ProblemReporter, SuperRefences uses this field. IProblem adds a field, ProblemReports use it. ThisReference changes a method and SuperRefence change too.</t>
+  </si>
+  <si>
+    <t>Lambda, Upsilon</t>
+  </si>
+  <si>
+    <t>FunctionalExpression-&gt;LambdaExpression-&gt;Parser,ThrowStatement,RenturnStatement</t>
+  </si>
+  <si>
+    <t>LocalVariableBinding changes one method, other classes: Argument, Sourcetypebing and aptSourceLocalVariabeBinding all changes</t>
+  </si>
+  <si>
+    <t>two parts: basemessageImpl-&gt;batchmessagerimpl and idemessagerimpl; annotatiionmembervalue-&gt;annotationmirrorimpl and executableElementImpl; basemessageimpl calls annotationmembervalue</t>
+  </si>
+  <si>
+    <t>Lambda; Domino; Pattern5</t>
+  </si>
+  <si>
+    <t>Classfileconstants, constant pool changes; other files use each one cochanges</t>
+  </si>
+  <si>
+    <t>2 lambda</t>
+  </si>
+  <si>
+    <t>Shift from tag bits to ivariablebinding; the following classes of these two cochanges</t>
+  </si>
+  <si>
+    <t>BindingKeyParser-&gt;BindingKeyResolver,JavaElementFinder; BindingKeyParser-&gt;CompilationUnitResolver; CharOperation-&gt;ModuleBinding</t>
+  </si>
+  <si>
+    <t>Because compilation use both bindingkeyparser and CharOperation</t>
+  </si>
+  <si>
+    <t>Lambda; Upsilon</t>
+  </si>
+  <si>
     <t>add method  in one class, other classes “call”,”extend” also add this method implementation</t>
   </si>
   <si>
+    <t>INameEnvironment delete one methods; other followers cochanges with it. a new class: InameenrionmentExtension created.</t>
+  </si>
+  <si>
+    <t>Lambda, Pattern5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BlockScope leads; other classes call it and change with it</t>
+  </si>
+  <si>
+    <t>methoddeclare-&gt;astconverter,naiveastflattener,defaultbindingresolver,astmatcher; abstractmethoddeclaration-&gt;methodscope</t>
+  </si>
+  <si>
     <t>Modify method parameter in one class; add parameter setting in another class; other class depends on first class now “call” bother classes</t>
+  </si>
+  <si>
+    <t>typebinding leads</t>
   </si>
   <si>
     <t>add  comments in one class, other classes “typed” also add similar comments</t>
@@ -113,7 +176,37 @@
     <t>two lead classes, one follow class, third layer classes and followers</t>
   </si>
   <si>
+    <t>Flowcontext leads; NullAnnotationMatching leads and problem reporter change</t>
+  </si>
+  <si>
+    <t>Lambda; Domino</t>
+  </si>
+  <si>
+    <t>IProblem and ProblemReasons lead the changes of ProblemReporter; local check logic in MessageSent extracted to BlockScope so Reference EXpresioon can also use it</t>
+  </si>
+  <si>
+    <t>Upsilon; Corn</t>
+  </si>
+  <si>
+    <t>InnerInferenceHelper leads; Invocation follows and other classes; two classes follows invocation</t>
+  </si>
+  <si>
+    <t>3 class adds constant and follower of each class changes</t>
+  </si>
+  <si>
+    <t>3 Lambda; Corn</t>
+  </si>
+  <si>
+    <t>Compiler and complieroptions changes and followers of these two cochanges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift from NdBinding to NdType; </t>
+  </si>
+  <si>
     <t>add one field in one class and one set method in another classes; other class depends on first class now “call” bother classes</t>
+  </si>
+  <si>
+    <t>typebinding -&gt; localtypebinding, scope-&gt;singletyperefence,blockscope,lambdaexpression</t>
   </si>
 </sst>
 </file>
@@ -146,7 +239,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +267,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -357,7 +456,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -406,11 +505,26 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,6 +550,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa4cde4"/>
+      <rgbColor rgb="ffff9690"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1530,7 +1645,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H527"/>
+  <dimension ref="A1:I527"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1544,7 +1659,8 @@
     <col min="6" max="6" width="46.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.6719" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.6719" style="1" customWidth="1"/>
-    <col min="9" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6719" style="1" customWidth="1"/>
+    <col min="10" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.85" customHeight="1">
@@ -1569,9 +1685,10 @@
       <c r="G1" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="6">
+      <c r="H1" t="s" s="5">
         <v>7</v>
       </c>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
       <c r="A2" s="7">
@@ -1592,6 +1709,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
       <c r="A3" s="10">
@@ -1618,6 +1736,7 @@
       <c r="H3" t="s" s="13">
         <v>10</v>
       </c>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
       <c r="A4" s="10">
@@ -1638,6 +1757,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="A5" s="10">
@@ -1658,6 +1778,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="A6" s="10">
@@ -1678,6 +1799,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="A7" s="10">
@@ -1698,6 +1820,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="A8" s="10">
@@ -1718,6 +1841,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" s="10">
@@ -1738,6 +1862,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="10">
@@ -1758,6 +1883,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" ht="27" customHeight="1">
       <c r="A11" s="10">
@@ -1784,6 +1910,7 @@
       <c r="H11" t="s" s="13">
         <v>13</v>
       </c>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="15">
@@ -1804,6 +1931,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="15">
@@ -1824,6 +1952,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="15">
@@ -1844,6 +1973,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="15">
@@ -1864,6 +1994,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="15">
@@ -1884,6 +2015,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="15">
@@ -1904,6 +2036,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" s="15">
@@ -1924,6 +2057,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" s="15">
@@ -1944,6 +2078,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
       <c r="A20" s="15">
@@ -1964,6 +2099,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
       <c r="A21" s="15">
@@ -1984,6 +2120,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
       <c r="A22" s="10">
@@ -2004,6 +2141,7 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
       <c r="A23" s="10">
@@ -2024,6 +2162,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" ht="20.35" customHeight="1">
       <c r="A24" s="10">
@@ -2044,6 +2183,7 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" ht="20.35" customHeight="1">
       <c r="A25" s="10">
@@ -2064,6 +2204,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" ht="20.35" customHeight="1">
       <c r="A26" s="10">
@@ -2084,6 +2225,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" ht="20.35" customHeight="1">
       <c r="A27" s="10">
@@ -2110,6 +2252,7 @@
       <c r="H27" t="s" s="13">
         <v>13</v>
       </c>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" ht="20.35" customHeight="1">
       <c r="A28" s="10">
@@ -2130,6 +2273,7 @@
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" ht="20.35" customHeight="1">
       <c r="A29" s="10">
@@ -2150,6 +2294,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" ht="20.35" customHeight="1">
       <c r="A30" s="10">
@@ -2170,6 +2315,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" ht="20.35" customHeight="1">
       <c r="A31" s="10">
@@ -2190,6 +2336,7 @@
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" ht="20.35" customHeight="1">
       <c r="A32" s="15">
@@ -2210,6 +2357,7 @@
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" ht="20.35" customHeight="1">
       <c r="A33" s="15">
@@ -2230,6 +2378,7 @@
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" ht="20.35" customHeight="1">
       <c r="A34" s="15">
@@ -2250,6 +2399,7 @@
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" ht="20.35" customHeight="1">
       <c r="A35" s="15">
@@ -2270,6 +2420,7 @@
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
       <c r="A36" s="15">
@@ -2290,6 +2441,7 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" ht="20.35" customHeight="1">
       <c r="A37" s="15">
@@ -2310,6 +2462,7 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" ht="20.35" customHeight="1">
       <c r="A38" s="15">
@@ -2336,6 +2489,7 @@
       <c r="H38" t="s" s="13">
         <v>16</v>
       </c>
+      <c r="I38" s="13"/>
     </row>
     <row r="39" ht="20.35" customHeight="1">
       <c r="A39" s="15">
@@ -2356,6 +2510,7 @@
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" ht="20.35" customHeight="1">
       <c r="A40" s="15">
@@ -2376,6 +2531,7 @@
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" ht="20.35" customHeight="1">
       <c r="A41" s="15">
@@ -2396,6 +2552,7 @@
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" ht="20.35" customHeight="1">
       <c r="A42" s="10">
@@ -2416,6 +2573,7 @@
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" ht="20.35" customHeight="1">
       <c r="A43" s="10">
@@ -2436,6 +2594,7 @@
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="20.35" customHeight="1">
       <c r="A44" s="10">
@@ -2456,6 +2615,7 @@
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
     </row>
     <row r="45" ht="20.35" customHeight="1">
       <c r="A45" s="10">
@@ -2476,6 +2636,7 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" ht="20.35" customHeight="1">
       <c r="A46" s="10">
@@ -2496,6 +2657,7 @@
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
     </row>
     <row r="47" ht="20.35" customHeight="1">
       <c r="A47" s="10">
@@ -2516,6 +2678,7 @@
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
     </row>
     <row r="48" ht="20.35" customHeight="1">
       <c r="A48" s="10">
@@ -2542,6 +2705,7 @@
       <c r="H48" t="s" s="13">
         <v>19</v>
       </c>
+      <c r="I48" s="13"/>
     </row>
     <row r="49" ht="20.35" customHeight="1">
       <c r="A49" s="10">
@@ -2562,6 +2726,7 @@
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
     </row>
     <row r="50" ht="20.35" customHeight="1">
       <c r="A50" s="10">
@@ -2582,6 +2747,7 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
     </row>
     <row r="51" ht="20.35" customHeight="1">
       <c r="A51" s="10">
@@ -2602,6 +2768,7 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
     </row>
     <row r="52" ht="20.35" customHeight="1">
       <c r="A52" s="15">
@@ -2622,6 +2789,7 @@
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
     </row>
     <row r="53" ht="20.35" customHeight="1">
       <c r="A53" s="15">
@@ -2642,6 +2810,7 @@
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
     </row>
     <row r="54" ht="20.35" customHeight="1">
       <c r="A54" s="15">
@@ -2662,6 +2831,7 @@
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
     </row>
     <row r="55" ht="20.35" customHeight="1">
       <c r="A55" s="15">
@@ -2682,6 +2852,7 @@
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
     </row>
     <row r="56" ht="20.35" customHeight="1">
       <c r="A56" s="15">
@@ -2702,6 +2873,7 @@
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
     </row>
     <row r="57" ht="20.35" customHeight="1">
       <c r="A57" s="15">
@@ -2722,6 +2894,7 @@
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
     </row>
     <row r="58" ht="20.35" customHeight="1">
       <c r="A58" s="15">
@@ -2748,6 +2921,7 @@
       <c r="H58" t="s" s="13">
         <v>22</v>
       </c>
+      <c r="I58" s="13"/>
     </row>
     <row r="59" ht="20.35" customHeight="1">
       <c r="A59" s="15">
@@ -2768,6 +2942,7 @@
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
     </row>
     <row r="60" ht="20.35" customHeight="1">
       <c r="A60" s="15">
@@ -2788,6 +2963,7 @@
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
     </row>
     <row r="61" ht="20.35" customHeight="1">
       <c r="A61" s="15">
@@ -2808,6 +2984,7 @@
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
     </row>
     <row r="62" ht="20.35" customHeight="1">
       <c r="A62" s="10">
@@ -2828,6 +3005,7 @@
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
     </row>
     <row r="63" ht="20.35" customHeight="1">
       <c r="A63" s="10">
@@ -2848,6 +3026,7 @@
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
     </row>
     <row r="64" ht="20.35" customHeight="1">
       <c r="A64" s="10">
@@ -2868,6 +3047,7 @@
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
     </row>
     <row r="65" ht="20.35" customHeight="1">
       <c r="A65" s="10">
@@ -2888,6 +3068,7 @@
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
     </row>
     <row r="66" ht="20.35" customHeight="1">
       <c r="A66" s="10">
@@ -2914,6 +3095,7 @@
       <c r="H66" t="s" s="13">
         <v>10</v>
       </c>
+      <c r="I66" s="13"/>
     </row>
     <row r="67" ht="20.35" customHeight="1">
       <c r="A67" s="10">
@@ -2934,6 +3116,7 @@
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
     </row>
     <row r="68" ht="20.35" customHeight="1">
       <c r="A68" s="10">
@@ -2954,6 +3137,7 @@
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
     </row>
     <row r="69" ht="20.35" customHeight="1">
       <c r="A69" s="10">
@@ -2974,6 +3158,7 @@
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
     </row>
     <row r="70" ht="20.35" customHeight="1">
       <c r="A70" s="10">
@@ -2994,6 +3179,7 @@
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
     </row>
     <row r="71" ht="20.35" customHeight="1">
       <c r="A71" s="10">
@@ -3014,6 +3200,7 @@
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
     </row>
     <row r="72" ht="20.35" customHeight="1">
       <c r="A72" s="15">
@@ -3034,6 +3221,7 @@
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
     </row>
     <row r="73" ht="20.35" customHeight="1">
       <c r="A73" s="15">
@@ -3054,6 +3242,7 @@
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
     </row>
     <row r="74" ht="20.35" customHeight="1">
       <c r="A74" s="15">
@@ -3074,6 +3263,7 @@
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
     </row>
     <row r="75" ht="20.35" customHeight="1">
       <c r="A75" s="15">
@@ -3094,6 +3284,7 @@
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
       <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
     </row>
     <row r="76" ht="20.35" customHeight="1">
       <c r="A76" s="15">
@@ -3114,6 +3305,7 @@
       <c r="F76" s="12"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
     </row>
     <row r="77" ht="20.35" customHeight="1">
       <c r="A77" s="15">
@@ -3134,6 +3326,7 @@
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
     </row>
     <row r="78" ht="20.35" customHeight="1">
       <c r="A78" s="15">
@@ -3154,6 +3347,7 @@
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
     </row>
     <row r="79" ht="20.35" customHeight="1">
       <c r="A79" s="15">
@@ -3180,6 +3374,7 @@
       <c r="H79" t="s" s="13">
         <v>27</v>
       </c>
+      <c r="I79" s="13"/>
     </row>
     <row r="80" ht="20.35" customHeight="1">
       <c r="A80" s="15">
@@ -3200,6 +3395,7 @@
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
     </row>
     <row r="81" ht="20.35" customHeight="1">
       <c r="A81" s="15">
@@ -3220,6 +3416,7 @@
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
     </row>
     <row r="82" ht="20.35" customHeight="1">
       <c r="A82" s="10">
@@ -3240,6 +3437,7 @@
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
     </row>
     <row r="83" ht="20.35" customHeight="1">
       <c r="A83" s="10">
@@ -3260,6 +3458,7 @@
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
     </row>
     <row r="84" ht="20.35" customHeight="1">
       <c r="A84" s="10">
@@ -3280,6 +3479,7 @@
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
     </row>
     <row r="85" ht="20.35" customHeight="1">
       <c r="A85" s="10">
@@ -3300,6 +3500,7 @@
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
     </row>
     <row r="86" ht="20.35" customHeight="1">
       <c r="A86" s="10">
@@ -3320,6 +3521,7 @@
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
     </row>
     <row r="87" ht="20.35" customHeight="1">
       <c r="A87" s="10">
@@ -3340,6 +3542,7 @@
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
     </row>
     <row r="88" ht="20.35" customHeight="1">
       <c r="A88" s="10">
@@ -3357,9 +3560,14 @@
       <c r="E88" s="12">
         <v>9</v>
       </c>
-      <c r="F88" s="12"/>
+      <c r="F88" t="s" s="13">
+        <v>28</v>
+      </c>
       <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
+      <c r="H88" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="I88" s="13"/>
     </row>
     <row r="89" ht="20.35" customHeight="1">
       <c r="A89" s="10">
@@ -3380,6 +3588,7 @@
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
     </row>
     <row r="90" ht="20.35" customHeight="1">
       <c r="A90" s="10">
@@ -3400,6 +3609,7 @@
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
     </row>
     <row r="91" ht="20.35" customHeight="1">
       <c r="A91" s="10">
@@ -3420,6 +3630,7 @@
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
     </row>
     <row r="92" ht="20.35" customHeight="1">
       <c r="A92" s="15">
@@ -3440,6 +3651,7 @@
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
     </row>
     <row r="93" ht="20.35" customHeight="1">
       <c r="A93" s="15">
@@ -3460,6 +3672,7 @@
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
     </row>
     <row r="94" ht="20.35" customHeight="1">
       <c r="A94" s="15">
@@ -3480,6 +3693,7 @@
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
     </row>
     <row r="95" ht="20.35" customHeight="1">
       <c r="A95" s="15">
@@ -3500,6 +3714,7 @@
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
     </row>
     <row r="96" ht="20.35" customHeight="1">
       <c r="A96" s="15">
@@ -3520,6 +3735,7 @@
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
     </row>
     <row r="97" ht="20.35" customHeight="1">
       <c r="A97" s="15">
@@ -3537,9 +3753,14 @@
       <c r="E97" s="12">
         <v>9</v>
       </c>
-      <c r="F97" s="12"/>
+      <c r="F97" t="s" s="13">
+        <v>29</v>
+      </c>
       <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
+      <c r="H97" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="I97" s="13"/>
     </row>
     <row r="98" ht="20.35" customHeight="1">
       <c r="A98" s="15">
@@ -3560,6 +3781,7 @@
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
     </row>
     <row r="99" ht="20.35" customHeight="1">
       <c r="A99" s="15">
@@ -3580,6 +3802,7 @@
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
     </row>
     <row r="100" ht="20.35" customHeight="1">
       <c r="A100" s="15">
@@ -3600,6 +3823,7 @@
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
     </row>
     <row r="101" ht="20.35" customHeight="1">
       <c r="A101" s="15">
@@ -3620,6 +3844,7 @@
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
+      <c r="I101" s="12"/>
     </row>
     <row r="102" ht="20.35" customHeight="1">
       <c r="A102" s="10">
@@ -3640,6 +3865,7 @@
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
+      <c r="I102" s="12"/>
     </row>
     <row r="103" ht="20.35" customHeight="1">
       <c r="A103" s="10">
@@ -3660,6 +3886,7 @@
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
+      <c r="I103" s="12"/>
     </row>
     <row r="104" ht="20.35" customHeight="1">
       <c r="A104" s="10">
@@ -3680,6 +3907,7 @@
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
+      <c r="I104" s="12"/>
     </row>
     <row r="105" ht="20.35" customHeight="1">
       <c r="A105" s="10">
@@ -3700,6 +3928,7 @@
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
+      <c r="I105" s="12"/>
     </row>
     <row r="106" ht="20.35" customHeight="1">
       <c r="A106" s="10">
@@ -3720,6 +3949,7 @@
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
+      <c r="I106" s="12"/>
     </row>
     <row r="107" ht="20.35" customHeight="1">
       <c r="A107" s="10">
@@ -3737,9 +3967,14 @@
       <c r="E107" s="12">
         <v>9</v>
       </c>
-      <c r="F107" s="12"/>
+      <c r="F107" t="s" s="13">
+        <v>31</v>
+      </c>
       <c r="G107" s="12"/>
-      <c r="H107" s="12"/>
+      <c r="H107" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="I107" s="13"/>
     </row>
     <row r="108" ht="20.35" customHeight="1">
       <c r="A108" s="10">
@@ -3760,6 +3995,7 @@
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
+      <c r="I108" s="12"/>
     </row>
     <row r="109" ht="20.35" customHeight="1">
       <c r="A109" s="10">
@@ -3780,6 +4016,7 @@
       <c r="F109" s="12"/>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
+      <c r="I109" s="12"/>
     </row>
     <row r="110" ht="20.35" customHeight="1">
       <c r="A110" s="10">
@@ -3800,6 +4037,7 @@
       <c r="F110" s="12"/>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
+      <c r="I110" s="12"/>
     </row>
     <row r="111" ht="20.35" customHeight="1">
       <c r="A111" s="10">
@@ -3820,6 +4058,7 @@
       <c r="F111" s="12"/>
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
+      <c r="I111" s="12"/>
     </row>
     <row r="112" ht="20.35" customHeight="1">
       <c r="A112" s="15">
@@ -3840,6 +4079,7 @@
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
+      <c r="I112" s="12"/>
     </row>
     <row r="113" ht="20.35" customHeight="1">
       <c r="A113" s="15">
@@ -3860,6 +4100,7 @@
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
+      <c r="I113" s="12"/>
     </row>
     <row r="114" ht="20.35" customHeight="1">
       <c r="A114" s="15">
@@ -3877,9 +4118,14 @@
       <c r="E114" s="12">
         <v>10</v>
       </c>
-      <c r="F114" s="12"/>
+      <c r="F114" t="s" s="13">
+        <v>32</v>
+      </c>
       <c r="G114" s="12"/>
-      <c r="H114" s="12"/>
+      <c r="H114" t="s" s="13">
+        <v>33</v>
+      </c>
+      <c r="I114" s="13"/>
     </row>
     <row r="115" ht="20.35" customHeight="1">
       <c r="A115" s="15">
@@ -3900,6 +4146,7 @@
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
+      <c r="I115" s="12"/>
     </row>
     <row r="116" ht="20.35" customHeight="1">
       <c r="A116" s="15">
@@ -3920,6 +4167,7 @@
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
       <c r="H116" s="12"/>
+      <c r="I116" s="12"/>
     </row>
     <row r="117" ht="20.35" customHeight="1">
       <c r="A117" s="15">
@@ -3940,6 +4188,7 @@
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
+      <c r="I117" s="12"/>
     </row>
     <row r="118" ht="20.35" customHeight="1">
       <c r="A118" s="15">
@@ -3960,6 +4209,7 @@
       <c r="F118" s="12"/>
       <c r="G118" s="12"/>
       <c r="H118" s="12"/>
+      <c r="I118" s="12"/>
     </row>
     <row r="119" ht="20.35" customHeight="1">
       <c r="A119" s="15">
@@ -3980,6 +4230,7 @@
       <c r="F119" s="12"/>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
+      <c r="I119" s="12"/>
     </row>
     <row r="120" ht="20.35" customHeight="1">
       <c r="A120" s="15">
@@ -4000,6 +4251,7 @@
       <c r="F120" s="12"/>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
+      <c r="I120" s="12"/>
     </row>
     <row r="121" ht="20.35" customHeight="1">
       <c r="A121" s="15">
@@ -4020,6 +4272,7 @@
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
+      <c r="I121" s="12"/>
     </row>
     <row r="122" ht="20.35" customHeight="1">
       <c r="A122" s="10">
@@ -4040,6 +4293,7 @@
       <c r="F122" s="12"/>
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
+      <c r="I122" s="12"/>
     </row>
     <row r="123" ht="20.35" customHeight="1">
       <c r="A123" s="10">
@@ -4060,6 +4314,7 @@
       <c r="F123" s="12"/>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
+      <c r="I123" s="12"/>
     </row>
     <row r="124" ht="20.35" customHeight="1">
       <c r="A124" s="10">
@@ -4080,6 +4335,7 @@
       <c r="F124" s="12"/>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
+      <c r="I124" s="12"/>
     </row>
     <row r="125" ht="20.35" customHeight="1">
       <c r="A125" s="10">
@@ -4097,9 +4353,14 @@
       <c r="E125" s="12">
         <v>10</v>
       </c>
-      <c r="F125" s="12"/>
+      <c r="F125" t="s" s="13">
+        <v>34</v>
+      </c>
       <c r="G125" s="12"/>
-      <c r="H125" s="12"/>
+      <c r="H125" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="I125" s="13"/>
     </row>
     <row r="126" ht="20.35" customHeight="1">
       <c r="A126" s="10">
@@ -4120,6 +4381,7 @@
       <c r="F126" s="12"/>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
+      <c r="I126" s="12"/>
     </row>
     <row r="127" ht="20.35" customHeight="1">
       <c r="A127" s="10">
@@ -4140,6 +4402,7 @@
       <c r="F127" s="12"/>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
+      <c r="I127" s="12"/>
     </row>
     <row r="128" ht="20.35" customHeight="1">
       <c r="A128" s="10">
@@ -4160,6 +4423,7 @@
       <c r="F128" s="12"/>
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
+      <c r="I128" s="12"/>
     </row>
     <row r="129" ht="20.35" customHeight="1">
       <c r="A129" s="10">
@@ -4180,6 +4444,7 @@
       <c r="F129" s="12"/>
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
+      <c r="I129" s="12"/>
     </row>
     <row r="130" ht="20.35" customHeight="1">
       <c r="A130" s="10">
@@ -4200,6 +4465,7 @@
       <c r="F130" s="12"/>
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
+      <c r="I130" s="12"/>
     </row>
     <row r="131" ht="20.35" customHeight="1">
       <c r="A131" s="10">
@@ -4220,6 +4486,7 @@
       <c r="F131" s="12"/>
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
+      <c r="I131" s="12"/>
     </row>
     <row r="132" ht="20.35" customHeight="1">
       <c r="A132" s="15">
@@ -4240,6 +4507,7 @@
       <c r="F132" s="12"/>
       <c r="G132" s="12"/>
       <c r="H132" s="12"/>
+      <c r="I132" s="12"/>
     </row>
     <row r="133" ht="20.35" customHeight="1">
       <c r="A133" s="15">
@@ -4260,6 +4528,7 @@
       <c r="F133" s="12"/>
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
+      <c r="I133" s="12"/>
     </row>
     <row r="134" ht="20.35" customHeight="1">
       <c r="A134" s="15">
@@ -4280,6 +4549,7 @@
       <c r="F134" s="12"/>
       <c r="G134" s="12"/>
       <c r="H134" s="12"/>
+      <c r="I134" s="12"/>
     </row>
     <row r="135" ht="20.35" customHeight="1">
       <c r="A135" s="15">
@@ -4300,6 +4570,7 @@
       <c r="F135" s="12"/>
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
+      <c r="I135" s="12"/>
     </row>
     <row r="136" ht="20.35" customHeight="1">
       <c r="A136" s="15">
@@ -4320,6 +4591,7 @@
       <c r="F136" s="12"/>
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
+      <c r="I136" s="12"/>
     </row>
     <row r="137" ht="20.35" customHeight="1">
       <c r="A137" s="15">
@@ -4340,6 +4612,7 @@
       <c r="F137" s="12"/>
       <c r="G137" s="12"/>
       <c r="H137" s="12"/>
+      <c r="I137" s="12"/>
     </row>
     <row r="138" ht="20.35" customHeight="1">
       <c r="A138" s="15">
@@ -4360,6 +4633,7 @@
       <c r="F138" s="12"/>
       <c r="G138" s="12"/>
       <c r="H138" s="12"/>
+      <c r="I138" s="12"/>
     </row>
     <row r="139" ht="20.35" customHeight="1">
       <c r="A139" s="15">
@@ -4380,6 +4654,7 @@
       <c r="F139" s="12"/>
       <c r="G139" s="12"/>
       <c r="H139" s="12"/>
+      <c r="I139" s="12"/>
     </row>
     <row r="140" ht="20.35" customHeight="1">
       <c r="A140" s="15">
@@ -4400,6 +4675,7 @@
       <c r="F140" s="12"/>
       <c r="G140" s="12"/>
       <c r="H140" s="12"/>
+      <c r="I140" s="12"/>
     </row>
     <row r="141" ht="20.35" customHeight="1">
       <c r="A141" s="15">
@@ -4417,9 +4693,14 @@
       <c r="E141" s="12">
         <v>11</v>
       </c>
-      <c r="F141" s="12"/>
+      <c r="F141" t="s" s="13">
+        <v>35</v>
+      </c>
       <c r="G141" s="12"/>
-      <c r="H141" s="12"/>
+      <c r="H141" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="I141" s="13"/>
     </row>
     <row r="142" ht="20.35" customHeight="1">
       <c r="A142" s="10">
@@ -4440,6 +4721,7 @@
       <c r="F142" s="12"/>
       <c r="G142" s="12"/>
       <c r="H142" s="12"/>
+      <c r="I142" s="12"/>
     </row>
     <row r="143" ht="20.35" customHeight="1">
       <c r="A143" s="10">
@@ -4460,6 +4742,7 @@
       <c r="F143" s="12"/>
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
+      <c r="I143" s="12"/>
     </row>
     <row r="144" ht="20.35" customHeight="1">
       <c r="A144" s="10">
@@ -4480,6 +4763,7 @@
       <c r="F144" s="12"/>
       <c r="G144" s="12"/>
       <c r="H144" s="12"/>
+      <c r="I144" s="12"/>
     </row>
     <row r="145" ht="20.35" customHeight="1">
       <c r="A145" s="10">
@@ -4500,6 +4784,7 @@
       <c r="F145" s="12"/>
       <c r="G145" s="12"/>
       <c r="H145" s="12"/>
+      <c r="I145" s="12"/>
     </row>
     <row r="146" ht="20.35" customHeight="1">
       <c r="A146" s="10">
@@ -4520,6 +4805,7 @@
       <c r="F146" s="12"/>
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
+      <c r="I146" s="12"/>
     </row>
     <row r="147" ht="20.35" customHeight="1">
       <c r="A147" s="10">
@@ -4540,6 +4826,7 @@
       <c r="F147" s="12"/>
       <c r="G147" s="12"/>
       <c r="H147" s="12"/>
+      <c r="I147" s="12"/>
     </row>
     <row r="148" ht="20.35" customHeight="1">
       <c r="A148" s="10">
@@ -4557,9 +4844,14 @@
       <c r="E148" s="12">
         <v>11</v>
       </c>
-      <c r="F148" s="12"/>
+      <c r="F148" t="s" s="13">
+        <v>36</v>
+      </c>
       <c r="G148" s="12"/>
-      <c r="H148" s="12"/>
+      <c r="H148" t="s" s="13">
+        <v>37</v>
+      </c>
+      <c r="I148" s="13"/>
     </row>
     <row r="149" ht="20.35" customHeight="1">
       <c r="A149" s="10">
@@ -4580,6 +4872,7 @@
       <c r="F149" s="12"/>
       <c r="G149" s="12"/>
       <c r="H149" s="12"/>
+      <c r="I149" s="12"/>
     </row>
     <row r="150" ht="20.35" customHeight="1">
       <c r="A150" s="10">
@@ -4600,6 +4893,7 @@
       <c r="F150" s="12"/>
       <c r="G150" s="12"/>
       <c r="H150" s="12"/>
+      <c r="I150" s="12"/>
     </row>
     <row r="151" ht="20.35" customHeight="1">
       <c r="A151" s="10">
@@ -4620,6 +4914,7 @@
       <c r="F151" s="12"/>
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
+      <c r="I151" s="12"/>
     </row>
     <row r="152" ht="20.35" customHeight="1">
       <c r="A152" s="15">
@@ -4640,6 +4935,7 @@
       <c r="F152" s="12"/>
       <c r="G152" s="12"/>
       <c r="H152" s="12"/>
+      <c r="I152" s="12"/>
     </row>
     <row r="153" ht="20.35" customHeight="1">
       <c r="A153" s="15">
@@ -4660,6 +4956,7 @@
       <c r="F153" s="12"/>
       <c r="G153" s="12"/>
       <c r="H153" s="12"/>
+      <c r="I153" s="12"/>
     </row>
     <row r="154" ht="20.35" customHeight="1">
       <c r="A154" s="15">
@@ -4680,6 +4977,7 @@
       <c r="F154" s="12"/>
       <c r="G154" s="12"/>
       <c r="H154" s="12"/>
+      <c r="I154" s="12"/>
     </row>
     <row r="155" ht="20.35" customHeight="1">
       <c r="A155" s="15">
@@ -4700,6 +4998,7 @@
       <c r="F155" s="12"/>
       <c r="G155" s="12"/>
       <c r="H155" s="12"/>
+      <c r="I155" s="12"/>
     </row>
     <row r="156" ht="20.35" customHeight="1">
       <c r="A156" s="15">
@@ -4720,6 +5019,7 @@
       <c r="F156" s="12"/>
       <c r="G156" s="12"/>
       <c r="H156" s="12"/>
+      <c r="I156" s="12"/>
     </row>
     <row r="157" ht="20.35" customHeight="1">
       <c r="A157" s="15">
@@ -4740,6 +5040,7 @@
       <c r="F157" s="12"/>
       <c r="G157" s="12"/>
       <c r="H157" s="12"/>
+      <c r="I157" s="12"/>
     </row>
     <row r="158" ht="20.35" customHeight="1">
       <c r="A158" s="15">
@@ -4757,9 +5058,14 @@
       <c r="E158" s="12">
         <v>12</v>
       </c>
-      <c r="F158" s="12"/>
+      <c r="F158" t="s" s="13">
+        <v>38</v>
+      </c>
       <c r="G158" s="12"/>
-      <c r="H158" s="12"/>
+      <c r="H158" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="I158" s="13"/>
     </row>
     <row r="159" ht="20.35" customHeight="1">
       <c r="A159" s="15">
@@ -4780,6 +5086,7 @@
       <c r="F159" s="12"/>
       <c r="G159" s="12"/>
       <c r="H159" s="12"/>
+      <c r="I159" s="12"/>
     </row>
     <row r="160" ht="20.35" customHeight="1">
       <c r="A160" s="15">
@@ -4800,6 +5107,7 @@
       <c r="F160" s="12"/>
       <c r="G160" s="12"/>
       <c r="H160" s="12"/>
+      <c r="I160" s="12"/>
     </row>
     <row r="161" ht="20.35" customHeight="1">
       <c r="A161" s="15">
@@ -4820,6 +5128,7 @@
       <c r="F161" s="12"/>
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
+      <c r="I161" s="12"/>
     </row>
     <row r="162" ht="20.35" customHeight="1">
       <c r="A162" s="10">
@@ -4840,6 +5149,7 @@
       <c r="F162" s="12"/>
       <c r="G162" s="12"/>
       <c r="H162" s="12"/>
+      <c r="I162" s="12"/>
     </row>
     <row r="163" ht="20.35" customHeight="1">
       <c r="A163" s="10">
@@ -4860,6 +5170,7 @@
       <c r="F163" s="12"/>
       <c r="G163" s="12"/>
       <c r="H163" s="12"/>
+      <c r="I163" s="12"/>
     </row>
     <row r="164" ht="20.35" customHeight="1">
       <c r="A164" s="10">
@@ -4877,9 +5188,14 @@
       <c r="E164" s="12">
         <v>12</v>
       </c>
-      <c r="F164" s="12"/>
+      <c r="F164" t="s" s="13">
+        <v>40</v>
+      </c>
       <c r="G164" s="12"/>
-      <c r="H164" s="12"/>
+      <c r="H164" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="I164" s="13"/>
     </row>
     <row r="165" ht="20.35" customHeight="1">
       <c r="A165" s="10">
@@ -4900,6 +5216,7 @@
       <c r="F165" s="12"/>
       <c r="G165" s="12"/>
       <c r="H165" s="12"/>
+      <c r="I165" s="12"/>
     </row>
     <row r="166" ht="20.35" customHeight="1">
       <c r="A166" s="10">
@@ -4920,6 +5237,7 @@
       <c r="F166" s="12"/>
       <c r="G166" s="12"/>
       <c r="H166" s="12"/>
+      <c r="I166" s="12"/>
     </row>
     <row r="167" ht="20.35" customHeight="1">
       <c r="A167" s="10">
@@ -4940,6 +5258,7 @@
       <c r="F167" s="12"/>
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
+      <c r="I167" s="12"/>
     </row>
     <row r="168" ht="20.35" customHeight="1">
       <c r="A168" s="10">
@@ -4960,6 +5279,7 @@
       <c r="F168" s="12"/>
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
     </row>
     <row r="169" ht="20.35" customHeight="1">
       <c r="A169" s="10">
@@ -4980,6 +5300,7 @@
       <c r="F169" s="12"/>
       <c r="G169" s="12"/>
       <c r="H169" s="12"/>
+      <c r="I169" s="12"/>
     </row>
     <row r="170" ht="20.35" customHeight="1">
       <c r="A170" s="10">
@@ -5000,6 +5321,7 @@
       <c r="F170" s="12"/>
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
+      <c r="I170" s="12"/>
     </row>
     <row r="171" ht="20.35" customHeight="1">
       <c r="A171" s="10">
@@ -5020,6 +5342,7 @@
       <c r="F171" s="12"/>
       <c r="G171" s="12"/>
       <c r="H171" s="12"/>
+      <c r="I171" s="12"/>
     </row>
     <row r="172" ht="20.35" customHeight="1">
       <c r="A172" s="15">
@@ -5040,6 +5363,7 @@
       <c r="F172" s="12"/>
       <c r="G172" s="12"/>
       <c r="H172" s="12"/>
+      <c r="I172" s="12"/>
     </row>
     <row r="173" ht="20.35" customHeight="1">
       <c r="A173" s="15">
@@ -5060,6 +5384,7 @@
       <c r="F173" s="12"/>
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
+      <c r="I173" s="12"/>
     </row>
     <row r="174" ht="20.35" customHeight="1">
       <c r="A174" s="15">
@@ -5080,6 +5405,7 @@
       <c r="F174" s="12"/>
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
+      <c r="I174" s="12"/>
     </row>
     <row r="175" ht="20.35" customHeight="1">
       <c r="A175" s="15">
@@ -5100,6 +5426,7 @@
       <c r="F175" s="12"/>
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
+      <c r="I175" s="12"/>
     </row>
     <row r="176" ht="20.35" customHeight="1">
       <c r="A176" s="15">
@@ -5120,6 +5447,7 @@
       <c r="F176" s="12"/>
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
+      <c r="I176" s="12"/>
     </row>
     <row r="177" ht="20.35" customHeight="1">
       <c r="A177" s="15">
@@ -5137,9 +5465,16 @@
       <c r="E177" s="12">
         <v>13</v>
       </c>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12"/>
-      <c r="H177" s="12"/>
+      <c r="F177" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="G177" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="H177" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="I177" s="13"/>
     </row>
     <row r="178" ht="20.35" customHeight="1">
       <c r="A178" s="15">
@@ -5160,6 +5495,7 @@
       <c r="F178" s="12"/>
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
+      <c r="I178" s="12"/>
     </row>
     <row r="179" ht="20.35" customHeight="1">
       <c r="A179" s="15">
@@ -5180,6 +5516,7 @@
       <c r="F179" s="12"/>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
+      <c r="I179" s="12"/>
     </row>
     <row r="180" ht="20.35" customHeight="1">
       <c r="A180" s="15">
@@ -5200,6 +5537,7 @@
       <c r="F180" s="12"/>
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
+      <c r="I180" s="12"/>
     </row>
     <row r="181" ht="20.35" customHeight="1">
       <c r="A181" s="15">
@@ -5220,6 +5558,7 @@
       <c r="F181" s="12"/>
       <c r="G181" s="12"/>
       <c r="H181" s="12"/>
+      <c r="I181" s="12"/>
     </row>
     <row r="182" ht="20.35" customHeight="1">
       <c r="A182" s="10">
@@ -5240,6 +5579,7 @@
       <c r="F182" s="12"/>
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
+      <c r="I182" s="12"/>
     </row>
     <row r="183" ht="20.35" customHeight="1">
       <c r="A183" s="10">
@@ -5260,6 +5600,7 @@
       <c r="F183" s="12"/>
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
+      <c r="I183" s="12"/>
     </row>
     <row r="184" ht="20.35" customHeight="1">
       <c r="A184" s="10">
@@ -5280,6 +5621,7 @@
       <c r="F184" s="12"/>
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
+      <c r="I184" s="12"/>
     </row>
     <row r="185" ht="20.35" customHeight="1">
       <c r="A185" s="10">
@@ -5300,6 +5642,7 @@
       <c r="F185" s="12"/>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
+      <c r="I185" s="12"/>
     </row>
     <row r="186" ht="20.35" customHeight="1">
       <c r="A186" s="10">
@@ -5320,6 +5663,7 @@
       <c r="F186" s="12"/>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
+      <c r="I186" s="12"/>
     </row>
     <row r="187" ht="20.35" customHeight="1">
       <c r="A187" s="10">
@@ -5340,6 +5684,7 @@
       <c r="F187" s="12"/>
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
+      <c r="I187" s="12"/>
     </row>
     <row r="188" ht="20.35" customHeight="1">
       <c r="A188" s="10">
@@ -5360,6 +5705,7 @@
       <c r="F188" s="12"/>
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
+      <c r="I188" s="12"/>
     </row>
     <row r="189" ht="20.35" customHeight="1">
       <c r="A189" s="10">
@@ -5380,6 +5726,7 @@
       <c r="F189" s="12"/>
       <c r="G189" s="12"/>
       <c r="H189" s="12"/>
+      <c r="I189" s="12"/>
     </row>
     <row r="190" ht="20.35" customHeight="1">
       <c r="A190" s="10">
@@ -5400,6 +5747,7 @@
       <c r="F190" s="12"/>
       <c r="G190" s="12"/>
       <c r="H190" s="12"/>
+      <c r="I190" s="12"/>
     </row>
     <row r="191" ht="20.35" customHeight="1">
       <c r="A191" s="10">
@@ -5418,7 +5766,7 @@
         <v>13</v>
       </c>
       <c r="F191" t="s" s="14">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G191" t="s" s="14">
         <v>12</v>
@@ -5426,6 +5774,7 @@
       <c r="H191" t="s" s="13">
         <v>16</v>
       </c>
+      <c r="I191" s="13"/>
     </row>
     <row r="192" ht="20.35" customHeight="1">
       <c r="A192" s="15">
@@ -5446,6 +5795,7 @@
       <c r="F192" s="12"/>
       <c r="G192" s="12"/>
       <c r="H192" s="12"/>
+      <c r="I192" s="12"/>
     </row>
     <row r="193" ht="20.35" customHeight="1">
       <c r="A193" s="15">
@@ -5466,6 +5816,7 @@
       <c r="F193" s="12"/>
       <c r="G193" s="12"/>
       <c r="H193" s="12"/>
+      <c r="I193" s="12"/>
     </row>
     <row r="194" ht="20.35" customHeight="1">
       <c r="A194" s="15">
@@ -5486,6 +5837,7 @@
       <c r="F194" s="12"/>
       <c r="G194" s="12"/>
       <c r="H194" s="12"/>
+      <c r="I194" s="12"/>
     </row>
     <row r="195" ht="20.35" customHeight="1">
       <c r="A195" s="15">
@@ -5506,6 +5858,7 @@
       <c r="F195" s="12"/>
       <c r="G195" s="12"/>
       <c r="H195" s="12"/>
+      <c r="I195" s="12"/>
     </row>
     <row r="196" ht="20.35" customHeight="1">
       <c r="A196" s="15">
@@ -5526,26 +5879,32 @@
       <c r="F196" s="12"/>
       <c r="G196" s="12"/>
       <c r="H196" s="12"/>
+      <c r="I196" s="12"/>
     </row>
     <row r="197" ht="20.35" customHeight="1">
-      <c r="A197" s="15">
+      <c r="A197" s="16">
         <v>493222</v>
       </c>
-      <c r="B197" s="11">
+      <c r="B197" s="17">
         <v>9</v>
       </c>
-      <c r="C197" s="12">
-        <v>1</v>
-      </c>
-      <c r="D197" s="12">
+      <c r="C197" s="18">
+        <v>1</v>
+      </c>
+      <c r="D197" s="18">
         <v>115</v>
       </c>
-      <c r="E197" s="12">
+      <c r="E197" s="18">
         <v>14</v>
       </c>
-      <c r="F197" s="12"/>
-      <c r="G197" s="12"/>
-      <c r="H197" s="12"/>
+      <c r="F197" t="s" s="19">
+        <v>45</v>
+      </c>
+      <c r="G197" s="18"/>
+      <c r="H197" t="s" s="19">
+        <v>46</v>
+      </c>
+      <c r="I197" s="19"/>
     </row>
     <row r="198" ht="20.35" customHeight="1">
       <c r="A198" s="15">
@@ -5566,6 +5925,7 @@
       <c r="F198" s="12"/>
       <c r="G198" s="12"/>
       <c r="H198" s="12"/>
+      <c r="I198" s="12"/>
     </row>
     <row r="199" ht="20.35" customHeight="1">
       <c r="A199" s="15">
@@ -5586,6 +5946,7 @@
       <c r="F199" s="12"/>
       <c r="G199" s="12"/>
       <c r="H199" s="12"/>
+      <c r="I199" s="12"/>
     </row>
     <row r="200" ht="20.35" customHeight="1">
       <c r="A200" s="15">
@@ -5606,6 +5967,7 @@
       <c r="F200" s="12"/>
       <c r="G200" s="12"/>
       <c r="H200" s="12"/>
+      <c r="I200" s="12"/>
     </row>
     <row r="201" ht="20.35" customHeight="1">
       <c r="A201" s="15">
@@ -5626,6 +5988,7 @@
       <c r="F201" s="12"/>
       <c r="G201" s="12"/>
       <c r="H201" s="12"/>
+      <c r="I201" s="12"/>
     </row>
     <row r="202" ht="20.35" customHeight="1">
       <c r="A202" s="10">
@@ -5646,6 +6009,7 @@
       <c r="F202" s="12"/>
       <c r="G202" s="12"/>
       <c r="H202" s="12"/>
+      <c r="I202" s="12"/>
     </row>
     <row r="203" ht="20.35" customHeight="1">
       <c r="A203" s="10">
@@ -5666,6 +6030,7 @@
       <c r="F203" s="12"/>
       <c r="G203" s="12"/>
       <c r="H203" s="12"/>
+      <c r="I203" s="12"/>
     </row>
     <row r="204" ht="20.35" customHeight="1">
       <c r="A204" s="10">
@@ -5686,6 +6051,7 @@
       <c r="F204" s="12"/>
       <c r="G204" s="12"/>
       <c r="H204" s="12"/>
+      <c r="I204" s="12"/>
     </row>
     <row r="205" ht="20.35" customHeight="1">
       <c r="A205" s="10">
@@ -5706,6 +6072,7 @@
       <c r="F205" s="12"/>
       <c r="G205" s="12"/>
       <c r="H205" s="12"/>
+      <c r="I205" s="12"/>
     </row>
     <row r="206" ht="20.35" customHeight="1">
       <c r="A206" s="10">
@@ -5723,9 +6090,14 @@
       <c r="E206" s="12">
         <v>14</v>
       </c>
-      <c r="F206" s="12"/>
+      <c r="F206" t="s" s="13">
+        <v>47</v>
+      </c>
       <c r="G206" s="12"/>
-      <c r="H206" s="12"/>
+      <c r="H206" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="I206" s="13"/>
     </row>
     <row r="207" ht="20.35" customHeight="1">
       <c r="A207" s="10">
@@ -5746,6 +6118,7 @@
       <c r="F207" s="12"/>
       <c r="G207" s="12"/>
       <c r="H207" s="12"/>
+      <c r="I207" s="12"/>
     </row>
     <row r="208" ht="20.35" customHeight="1">
       <c r="A208" s="10">
@@ -5766,6 +6139,7 @@
       <c r="F208" s="12"/>
       <c r="G208" s="12"/>
       <c r="H208" s="12"/>
+      <c r="I208" s="12"/>
     </row>
     <row r="209" ht="20.35" customHeight="1">
       <c r="A209" s="10">
@@ -5786,6 +6160,7 @@
       <c r="F209" s="12"/>
       <c r="G209" s="12"/>
       <c r="H209" s="12"/>
+      <c r="I209" s="12"/>
     </row>
     <row r="210" ht="20.35" customHeight="1">
       <c r="A210" s="10">
@@ -5806,6 +6181,7 @@
       <c r="F210" s="12"/>
       <c r="G210" s="12"/>
       <c r="H210" s="12"/>
+      <c r="I210" s="12"/>
     </row>
     <row r="211" ht="20.35" customHeight="1">
       <c r="A211" s="10">
@@ -5826,6 +6202,7 @@
       <c r="F211" s="12"/>
       <c r="G211" s="12"/>
       <c r="H211" s="12"/>
+      <c r="I211" s="12"/>
     </row>
     <row r="212" ht="20.35" customHeight="1">
       <c r="A212" s="15">
@@ -5846,6 +6223,7 @@
       <c r="F212" s="12"/>
       <c r="G212" s="12"/>
       <c r="H212" s="12"/>
+      <c r="I212" s="12"/>
     </row>
     <row r="213" ht="20.35" customHeight="1">
       <c r="A213" s="15">
@@ -5866,6 +6244,7 @@
       <c r="F213" s="12"/>
       <c r="G213" s="12"/>
       <c r="H213" s="12"/>
+      <c r="I213" s="12"/>
     </row>
     <row r="214" ht="20.35" customHeight="1">
       <c r="A214" s="15">
@@ -5886,6 +6265,7 @@
       <c r="F214" s="12"/>
       <c r="G214" s="12"/>
       <c r="H214" s="12"/>
+      <c r="I214" s="12"/>
     </row>
     <row r="215" ht="20.35" customHeight="1">
       <c r="A215" s="15">
@@ -5906,6 +6286,7 @@
       <c r="F215" s="12"/>
       <c r="G215" s="12"/>
       <c r="H215" s="12"/>
+      <c r="I215" s="12"/>
     </row>
     <row r="216" ht="20.35" customHeight="1">
       <c r="A216" s="15">
@@ -5926,6 +6307,7 @@
       <c r="F216" s="12"/>
       <c r="G216" s="12"/>
       <c r="H216" s="12"/>
+      <c r="I216" s="12"/>
     </row>
     <row r="217" ht="20.35" customHeight="1">
       <c r="A217" s="15">
@@ -5943,9 +6325,14 @@
       <c r="E217" s="12">
         <v>15</v>
       </c>
-      <c r="F217" s="12"/>
+      <c r="F217" t="s" s="13">
+        <v>48</v>
+      </c>
       <c r="G217" s="12"/>
-      <c r="H217" s="12"/>
+      <c r="H217" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="I217" s="13"/>
     </row>
     <row r="218" ht="20.35" customHeight="1">
       <c r="A218" s="15">
@@ -5966,6 +6353,7 @@
       <c r="F218" s="12"/>
       <c r="G218" s="12"/>
       <c r="H218" s="12"/>
+      <c r="I218" s="12"/>
     </row>
     <row r="219" ht="20.35" customHeight="1">
       <c r="A219" s="15">
@@ -5986,6 +6374,7 @@
       <c r="F219" s="12"/>
       <c r="G219" s="12"/>
       <c r="H219" s="12"/>
+      <c r="I219" s="12"/>
     </row>
     <row r="220" ht="20.35" customHeight="1">
       <c r="A220" s="15">
@@ -6006,6 +6395,7 @@
       <c r="F220" s="12"/>
       <c r="G220" s="12"/>
       <c r="H220" s="12"/>
+      <c r="I220" s="12"/>
     </row>
     <row r="221" ht="20.35" customHeight="1">
       <c r="A221" s="15">
@@ -6026,6 +6416,7 @@
       <c r="F221" s="12"/>
       <c r="G221" s="12"/>
       <c r="H221" s="12"/>
+      <c r="I221" s="12"/>
     </row>
     <row r="222" ht="20.35" customHeight="1">
       <c r="A222" s="10">
@@ -6046,6 +6437,7 @@
       <c r="F222" s="12"/>
       <c r="G222" s="12"/>
       <c r="H222" s="12"/>
+      <c r="I222" s="12"/>
     </row>
     <row r="223" ht="20.35" customHeight="1">
       <c r="A223" s="10">
@@ -6066,6 +6458,7 @@
       <c r="F223" s="12"/>
       <c r="G223" s="12"/>
       <c r="H223" s="12"/>
+      <c r="I223" s="12"/>
     </row>
     <row r="224" ht="20.35" customHeight="1">
       <c r="A224" s="10">
@@ -6086,6 +6479,7 @@
       <c r="F224" s="12"/>
       <c r="G224" s="12"/>
       <c r="H224" s="12"/>
+      <c r="I224" s="12"/>
     </row>
     <row r="225" ht="20.35" customHeight="1">
       <c r="A225" s="10">
@@ -6106,6 +6500,7 @@
       <c r="F225" s="12"/>
       <c r="G225" s="12"/>
       <c r="H225" s="12"/>
+      <c r="I225" s="12"/>
     </row>
     <row r="226" ht="20.35" customHeight="1">
       <c r="A226" s="10">
@@ -6126,6 +6521,7 @@
       <c r="F226" s="12"/>
       <c r="G226" s="12"/>
       <c r="H226" s="12"/>
+      <c r="I226" s="12"/>
     </row>
     <row r="227" ht="46.25" customHeight="1">
       <c r="A227" s="10">
@@ -6144,7 +6540,7 @@
         <v>16</v>
       </c>
       <c r="F227" t="s" s="14">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G227" t="s" s="14">
         <v>18</v>
@@ -6152,6 +6548,7 @@
       <c r="H227" t="s" s="13">
         <v>27</v>
       </c>
+      <c r="I227" s="13"/>
     </row>
     <row r="228" ht="20.35" customHeight="1">
       <c r="A228" s="10">
@@ -6172,6 +6569,7 @@
       <c r="F228" s="12"/>
       <c r="G228" s="12"/>
       <c r="H228" s="12"/>
+      <c r="I228" s="12"/>
     </row>
     <row r="229" ht="20.35" customHeight="1">
       <c r="A229" s="10">
@@ -6192,6 +6590,7 @@
       <c r="F229" s="12"/>
       <c r="G229" s="12"/>
       <c r="H229" s="12"/>
+      <c r="I229" s="12"/>
     </row>
     <row r="230" ht="20.35" customHeight="1">
       <c r="A230" s="10">
@@ -6212,6 +6611,7 @@
       <c r="F230" s="12"/>
       <c r="G230" s="12"/>
       <c r="H230" s="12"/>
+      <c r="I230" s="12"/>
     </row>
     <row r="231" ht="20.35" customHeight="1">
       <c r="A231" s="10">
@@ -6232,6 +6632,7 @@
       <c r="F231" s="12"/>
       <c r="G231" s="12"/>
       <c r="H231" s="12"/>
+      <c r="I231" s="12"/>
     </row>
     <row r="232" ht="20.35" customHeight="1">
       <c r="A232" s="15">
@@ -6252,6 +6653,7 @@
       <c r="F232" s="12"/>
       <c r="G232" s="12"/>
       <c r="H232" s="12"/>
+      <c r="I232" s="12"/>
     </row>
     <row r="233" ht="20.35" customHeight="1">
       <c r="A233" s="15">
@@ -6272,6 +6674,7 @@
       <c r="F233" s="12"/>
       <c r="G233" s="12"/>
       <c r="H233" s="12"/>
+      <c r="I233" s="12"/>
     </row>
     <row r="234" ht="20.35" customHeight="1">
       <c r="A234" s="15">
@@ -6292,6 +6695,7 @@
       <c r="F234" s="12"/>
       <c r="G234" s="12"/>
       <c r="H234" s="12"/>
+      <c r="I234" s="12"/>
     </row>
     <row r="235" ht="20.35" customHeight="1">
       <c r="A235" s="15">
@@ -6312,6 +6716,7 @@
       <c r="F235" s="12"/>
       <c r="G235" s="12"/>
       <c r="H235" s="12"/>
+      <c r="I235" s="12"/>
     </row>
     <row r="236" ht="20.35" customHeight="1">
       <c r="A236" s="15">
@@ -6332,6 +6737,7 @@
       <c r="F236" s="12"/>
       <c r="G236" s="12"/>
       <c r="H236" s="12"/>
+      <c r="I236" s="12"/>
     </row>
     <row r="237" ht="20.35" customHeight="1">
       <c r="A237" s="15">
@@ -6349,9 +6755,14 @@
       <c r="E237" s="12">
         <v>17</v>
       </c>
-      <c r="F237" s="12"/>
+      <c r="F237" t="s" s="13">
+        <v>50</v>
+      </c>
       <c r="G237" s="12"/>
-      <c r="H237" s="12"/>
+      <c r="H237" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="I237" s="12"/>
     </row>
     <row r="238" ht="20.35" customHeight="1">
       <c r="A238" s="15">
@@ -6372,6 +6783,7 @@
       <c r="F238" s="12"/>
       <c r="G238" s="12"/>
       <c r="H238" s="12"/>
+      <c r="I238" s="12"/>
     </row>
     <row r="239" ht="20.35" customHeight="1">
       <c r="A239" s="15">
@@ -6392,6 +6804,7 @@
       <c r="F239" s="12"/>
       <c r="G239" s="12"/>
       <c r="H239" s="12"/>
+      <c r="I239" s="12"/>
     </row>
     <row r="240" ht="20.35" customHeight="1">
       <c r="A240" s="15">
@@ -6412,6 +6825,7 @@
       <c r="F240" s="12"/>
       <c r="G240" s="12"/>
       <c r="H240" s="12"/>
+      <c r="I240" s="12"/>
     </row>
     <row r="241" ht="20.35" customHeight="1">
       <c r="A241" s="15">
@@ -6432,6 +6846,7 @@
       <c r="F241" s="12"/>
       <c r="G241" s="12"/>
       <c r="H241" s="12"/>
+      <c r="I241" s="12"/>
     </row>
     <row r="242" ht="20.35" customHeight="1">
       <c r="A242" s="10">
@@ -6449,9 +6864,10 @@
       <c r="E242" s="12">
         <v>17</v>
       </c>
-      <c r="F242" s="16"/>
-      <c r="G242" s="16"/>
+      <c r="F242" s="20"/>
+      <c r="G242" s="20"/>
       <c r="H242" s="12"/>
+      <c r="I242" s="12"/>
     </row>
     <row r="243" ht="20.35" customHeight="1">
       <c r="A243" s="10">
@@ -6469,15 +6885,16 @@
       <c r="E243" s="12">
         <v>17</v>
       </c>
-      <c r="F243" t="s" s="17">
-        <v>30</v>
-      </c>
-      <c r="G243" t="s" s="17">
+      <c r="F243" t="s" s="21">
+        <v>51</v>
+      </c>
+      <c r="G243" t="s" s="21">
         <v>12</v>
       </c>
       <c r="H243" t="s" s="13">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I243" s="13"/>
     </row>
     <row r="244" ht="20.35" customHeight="1">
       <c r="A244" s="10">
@@ -6498,6 +6915,7 @@
       <c r="F244" s="12"/>
       <c r="G244" s="12"/>
       <c r="H244" s="12"/>
+      <c r="I244" s="12"/>
     </row>
     <row r="245" ht="20.35" customHeight="1">
       <c r="A245" s="10">
@@ -6518,6 +6936,7 @@
       <c r="F245" s="12"/>
       <c r="G245" s="12"/>
       <c r="H245" s="12"/>
+      <c r="I245" s="12"/>
     </row>
     <row r="246" ht="20.35" customHeight="1">
       <c r="A246" s="10">
@@ -6538,6 +6957,7 @@
       <c r="F246" s="12"/>
       <c r="G246" s="12"/>
       <c r="H246" s="12"/>
+      <c r="I246" s="12"/>
     </row>
     <row r="247" ht="20.35" customHeight="1">
       <c r="A247" s="10">
@@ -6558,6 +6978,7 @@
       <c r="F247" s="12"/>
       <c r="G247" s="12"/>
       <c r="H247" s="12"/>
+      <c r="I247" s="12"/>
     </row>
     <row r="248" ht="20.35" customHeight="1">
       <c r="A248" s="10">
@@ -6578,6 +6999,7 @@
       <c r="F248" s="12"/>
       <c r="G248" s="12"/>
       <c r="H248" s="12"/>
+      <c r="I248" s="12"/>
     </row>
     <row r="249" ht="20.35" customHeight="1">
       <c r="A249" s="10">
@@ -6598,6 +7020,7 @@
       <c r="F249" s="12"/>
       <c r="G249" s="12"/>
       <c r="H249" s="12"/>
+      <c r="I249" s="12"/>
     </row>
     <row r="250" ht="20.35" customHeight="1">
       <c r="A250" s="10">
@@ -6618,6 +7041,7 @@
       <c r="F250" s="12"/>
       <c r="G250" s="12"/>
       <c r="H250" s="12"/>
+      <c r="I250" s="12"/>
     </row>
     <row r="251" ht="20.35" customHeight="1">
       <c r="A251" s="10">
@@ -6638,6 +7062,7 @@
       <c r="F251" s="12"/>
       <c r="G251" s="12"/>
       <c r="H251" s="12"/>
+      <c r="I251" s="12"/>
     </row>
     <row r="252" ht="20.35" customHeight="1">
       <c r="A252" s="15">
@@ -6658,6 +7083,7 @@
       <c r="F252" s="12"/>
       <c r="G252" s="12"/>
       <c r="H252" s="12"/>
+      <c r="I252" s="12"/>
     </row>
     <row r="253" ht="20.35" customHeight="1">
       <c r="A253" s="15">
@@ -6678,6 +7104,7 @@
       <c r="F253" s="12"/>
       <c r="G253" s="12"/>
       <c r="H253" s="12"/>
+      <c r="I253" s="12"/>
     </row>
     <row r="254" ht="20.35" customHeight="1">
       <c r="A254" s="15">
@@ -6698,6 +7125,7 @@
       <c r="F254" s="12"/>
       <c r="G254" s="12"/>
       <c r="H254" s="12"/>
+      <c r="I254" s="12"/>
     </row>
     <row r="255" ht="20.35" customHeight="1">
       <c r="A255" s="15">
@@ -6716,14 +7144,15 @@
         <v>18</v>
       </c>
       <c r="F255" t="s" s="14">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G255" t="s" s="14">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="H255" t="s" s="13">
         <v>22</v>
       </c>
+      <c r="I255" s="13"/>
     </row>
     <row r="256" ht="20.35" customHeight="1">
       <c r="A256" s="15">
@@ -6744,6 +7173,7 @@
       <c r="F256" s="12"/>
       <c r="G256" s="12"/>
       <c r="H256" s="12"/>
+      <c r="I256" s="12"/>
     </row>
     <row r="257" ht="20.35" customHeight="1">
       <c r="A257" s="15">
@@ -6764,6 +7194,7 @@
       <c r="F257" s="12"/>
       <c r="G257" s="12"/>
       <c r="H257" s="12"/>
+      <c r="I257" s="12"/>
     </row>
     <row r="258" ht="20.35" customHeight="1">
       <c r="A258" s="15">
@@ -6784,6 +7215,7 @@
       <c r="F258" s="12"/>
       <c r="G258" s="12"/>
       <c r="H258" s="12"/>
+      <c r="I258" s="12"/>
     </row>
     <row r="259" ht="20.35" customHeight="1">
       <c r="A259" s="15">
@@ -6804,6 +7236,7 @@
       <c r="F259" s="12"/>
       <c r="G259" s="12"/>
       <c r="H259" s="12"/>
+      <c r="I259" s="12"/>
     </row>
     <row r="260" ht="20.35" customHeight="1">
       <c r="A260" s="15">
@@ -6824,6 +7257,7 @@
       <c r="F260" s="12"/>
       <c r="G260" s="12"/>
       <c r="H260" s="12"/>
+      <c r="I260" s="12"/>
     </row>
     <row r="261" ht="20.35" customHeight="1">
       <c r="A261" s="15">
@@ -6844,6 +7278,7 @@
       <c r="F261" s="12"/>
       <c r="G261" s="12"/>
       <c r="H261" s="12"/>
+      <c r="I261" s="12"/>
     </row>
     <row r="262" ht="20.35" customHeight="1">
       <c r="A262" s="10">
@@ -6864,6 +7299,7 @@
       <c r="F262" s="12"/>
       <c r="G262" s="12"/>
       <c r="H262" s="12"/>
+      <c r="I262" s="12"/>
     </row>
     <row r="263" ht="20.35" customHeight="1">
       <c r="A263" s="10">
@@ -6884,6 +7320,7 @@
       <c r="F263" s="12"/>
       <c r="G263" s="12"/>
       <c r="H263" s="12"/>
+      <c r="I263" s="12"/>
     </row>
     <row r="264" ht="20.35" customHeight="1">
       <c r="A264" s="10">
@@ -6904,6 +7341,7 @@
       <c r="F264" s="12"/>
       <c r="G264" s="12"/>
       <c r="H264" s="12"/>
+      <c r="I264" s="12"/>
     </row>
     <row r="265" ht="20.35" customHeight="1">
       <c r="A265" s="10">
@@ -6924,6 +7362,7 @@
       <c r="F265" s="12"/>
       <c r="G265" s="12"/>
       <c r="H265" s="12"/>
+      <c r="I265" s="12"/>
     </row>
     <row r="266" ht="20.35" customHeight="1">
       <c r="A266" s="10">
@@ -6944,6 +7383,7 @@
       <c r="F266" s="12"/>
       <c r="G266" s="12"/>
       <c r="H266" s="12"/>
+      <c r="I266" s="12"/>
     </row>
     <row r="267" ht="20.35" customHeight="1">
       <c r="A267" s="10">
@@ -6964,6 +7404,7 @@
       <c r="F267" s="12"/>
       <c r="G267" s="12"/>
       <c r="H267" s="12"/>
+      <c r="I267" s="12"/>
     </row>
     <row r="268" ht="20.35" customHeight="1">
       <c r="A268" s="10">
@@ -6981,9 +7422,14 @@
       <c r="E268" s="12">
         <v>20</v>
       </c>
-      <c r="F268" s="12"/>
+      <c r="F268" t="s" s="13">
+        <v>54</v>
+      </c>
       <c r="G268" s="12"/>
-      <c r="H268" s="12"/>
+      <c r="H268" t="s" s="13">
+        <v>55</v>
+      </c>
+      <c r="I268" s="12"/>
     </row>
     <row r="269" ht="20.35" customHeight="1">
       <c r="A269" s="10">
@@ -7004,6 +7450,7 @@
       <c r="F269" s="12"/>
       <c r="G269" s="12"/>
       <c r="H269" s="12"/>
+      <c r="I269" s="12"/>
     </row>
     <row r="270" ht="20.35" customHeight="1">
       <c r="A270" s="10">
@@ -7024,6 +7471,7 @@
       <c r="F270" s="12"/>
       <c r="G270" s="12"/>
       <c r="H270" s="12"/>
+      <c r="I270" s="12"/>
     </row>
     <row r="271" ht="20.35" customHeight="1">
       <c r="A271" s="10">
@@ -7044,6 +7492,7 @@
       <c r="F271" s="12"/>
       <c r="G271" s="12"/>
       <c r="H271" s="12"/>
+      <c r="I271" s="12"/>
     </row>
     <row r="272" ht="20.35" customHeight="1">
       <c r="A272" s="15">
@@ -7064,6 +7513,7 @@
       <c r="F272" s="12"/>
       <c r="G272" s="12"/>
       <c r="H272" s="12"/>
+      <c r="I272" s="12"/>
     </row>
     <row r="273" ht="20.35" customHeight="1">
       <c r="A273" s="15">
@@ -7084,6 +7534,7 @@
       <c r="F273" s="12"/>
       <c r="G273" s="12"/>
       <c r="H273" s="12"/>
+      <c r="I273" s="12"/>
     </row>
     <row r="274" ht="20.35" customHeight="1">
       <c r="A274" s="15">
@@ -7104,6 +7555,7 @@
       <c r="F274" s="12"/>
       <c r="G274" s="12"/>
       <c r="H274" s="12"/>
+      <c r="I274" s="12"/>
     </row>
     <row r="275" ht="20.35" customHeight="1">
       <c r="A275" s="15">
@@ -7124,6 +7576,7 @@
       <c r="F275" s="12"/>
       <c r="G275" s="12"/>
       <c r="H275" s="12"/>
+      <c r="I275" s="12"/>
     </row>
     <row r="276" ht="20.35" customHeight="1">
       <c r="A276" s="15">
@@ -7144,26 +7597,32 @@
       <c r="F276" s="12"/>
       <c r="G276" s="12"/>
       <c r="H276" s="12"/>
+      <c r="I276" s="12"/>
     </row>
     <row r="277" ht="20.35" customHeight="1">
-      <c r="A277" s="15">
+      <c r="A277" s="16">
         <v>404649</v>
       </c>
-      <c r="B277" s="11">
+      <c r="B277" s="17">
         <v>8</v>
       </c>
-      <c r="C277" s="12">
+      <c r="C277" s="18">
         <v>3</v>
       </c>
-      <c r="D277" s="12">
+      <c r="D277" s="18">
         <v>275</v>
       </c>
-      <c r="E277" s="12">
+      <c r="E277" s="18">
         <v>21</v>
       </c>
-      <c r="F277" s="12"/>
-      <c r="G277" s="12"/>
-      <c r="H277" s="12"/>
+      <c r="F277" t="s" s="19">
+        <v>56</v>
+      </c>
+      <c r="G277" s="18"/>
+      <c r="H277" t="s" s="19">
+        <v>57</v>
+      </c>
+      <c r="I277" s="18"/>
     </row>
     <row r="278" ht="20.35" customHeight="1">
       <c r="A278" s="15">
@@ -7184,6 +7643,7 @@
       <c r="F278" s="12"/>
       <c r="G278" s="12"/>
       <c r="H278" s="12"/>
+      <c r="I278" s="12"/>
     </row>
     <row r="279" ht="20.35" customHeight="1">
       <c r="A279" s="15">
@@ -7204,6 +7664,7 @@
       <c r="F279" s="12"/>
       <c r="G279" s="12"/>
       <c r="H279" s="12"/>
+      <c r="I279" s="12"/>
     </row>
     <row r="280" ht="20.35" customHeight="1">
       <c r="A280" s="15">
@@ -7224,6 +7685,7 @@
       <c r="F280" s="12"/>
       <c r="G280" s="12"/>
       <c r="H280" s="12"/>
+      <c r="I280" s="12"/>
     </row>
     <row r="281" ht="20.35" customHeight="1">
       <c r="A281" s="15">
@@ -7244,6 +7706,7 @@
       <c r="F281" s="12"/>
       <c r="G281" s="12"/>
       <c r="H281" s="12"/>
+      <c r="I281" s="12"/>
     </row>
     <row r="282" ht="20.35" customHeight="1">
       <c r="A282" s="10">
@@ -7264,6 +7727,7 @@
       <c r="F282" s="12"/>
       <c r="G282" s="12"/>
       <c r="H282" s="12"/>
+      <c r="I282" s="12"/>
     </row>
     <row r="283" ht="20.35" customHeight="1">
       <c r="A283" s="10">
@@ -7284,6 +7748,7 @@
       <c r="F283" s="12"/>
       <c r="G283" s="12"/>
       <c r="H283" s="12"/>
+      <c r="I283" s="12"/>
     </row>
     <row r="284" ht="20.35" customHeight="1">
       <c r="A284" s="10">
@@ -7304,6 +7769,7 @@
       <c r="F284" s="12"/>
       <c r="G284" s="12"/>
       <c r="H284" s="12"/>
+      <c r="I284" s="12"/>
     </row>
     <row r="285" ht="20.35" customHeight="1">
       <c r="A285" s="10">
@@ -7324,6 +7790,7 @@
       <c r="F285" s="12"/>
       <c r="G285" s="12"/>
       <c r="H285" s="12"/>
+      <c r="I285" s="12"/>
     </row>
     <row r="286" ht="20.35" customHeight="1">
       <c r="A286" s="10">
@@ -7341,9 +7808,14 @@
       <c r="E286" s="12">
         <v>22</v>
       </c>
-      <c r="F286" s="12"/>
+      <c r="F286" t="s" s="13">
+        <v>58</v>
+      </c>
       <c r="G286" s="12"/>
-      <c r="H286" s="12"/>
+      <c r="H286" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="I286" s="12"/>
     </row>
     <row r="287" ht="20.35" customHeight="1">
       <c r="A287" s="10">
@@ -7364,6 +7836,7 @@
       <c r="F287" s="12"/>
       <c r="G287" s="12"/>
       <c r="H287" s="12"/>
+      <c r="I287" s="12"/>
     </row>
     <row r="288" ht="20.35" customHeight="1">
       <c r="A288" s="10">
@@ -7384,6 +7857,7 @@
       <c r="F288" s="12"/>
       <c r="G288" s="12"/>
       <c r="H288" s="12"/>
+      <c r="I288" s="12"/>
     </row>
     <row r="289" ht="20.35" customHeight="1">
       <c r="A289" s="10">
@@ -7404,6 +7878,7 @@
       <c r="F289" s="12"/>
       <c r="G289" s="12"/>
       <c r="H289" s="12"/>
+      <c r="I289" s="12"/>
     </row>
     <row r="290" ht="20.35" customHeight="1">
       <c r="A290" s="10">
@@ -7424,6 +7899,7 @@
       <c r="F290" s="12"/>
       <c r="G290" s="12"/>
       <c r="H290" s="12"/>
+      <c r="I290" s="12"/>
     </row>
     <row r="291" ht="20.35" customHeight="1">
       <c r="A291" s="10">
@@ -7444,6 +7920,7 @@
       <c r="F291" s="12"/>
       <c r="G291" s="12"/>
       <c r="H291" s="12"/>
+      <c r="I291" s="12"/>
     </row>
     <row r="292" ht="20.35" customHeight="1">
       <c r="A292" s="15">
@@ -7464,6 +7941,7 @@
       <c r="F292" s="12"/>
       <c r="G292" s="12"/>
       <c r="H292" s="12"/>
+      <c r="I292" s="12"/>
     </row>
     <row r="293" ht="20.35" customHeight="1">
       <c r="A293" s="15">
@@ -7484,6 +7962,7 @@
       <c r="F293" s="12"/>
       <c r="G293" s="12"/>
       <c r="H293" s="12"/>
+      <c r="I293" s="12"/>
     </row>
     <row r="294" ht="20.35" customHeight="1">
       <c r="A294" s="15">
@@ -7504,6 +7983,7 @@
       <c r="F294" s="12"/>
       <c r="G294" s="12"/>
       <c r="H294" s="12"/>
+      <c r="I294" s="12"/>
     </row>
     <row r="295" ht="20.35" customHeight="1">
       <c r="A295" s="15">
@@ -7524,6 +8004,7 @@
       <c r="F295" s="12"/>
       <c r="G295" s="12"/>
       <c r="H295" s="12"/>
+      <c r="I295" s="12"/>
     </row>
     <row r="296" ht="20.35" customHeight="1">
       <c r="A296" s="15">
@@ -7544,6 +8025,7 @@
       <c r="F296" s="12"/>
       <c r="G296" s="12"/>
       <c r="H296" s="12"/>
+      <c r="I296" s="12"/>
     </row>
     <row r="297" ht="20.35" customHeight="1">
       <c r="A297" s="15">
@@ -7561,9 +8043,14 @@
       <c r="E297" s="12">
         <v>23</v>
       </c>
-      <c r="F297" s="12"/>
+      <c r="F297" t="s" s="13">
+        <v>59</v>
+      </c>
       <c r="G297" s="12"/>
-      <c r="H297" s="12"/>
+      <c r="H297" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="I297" s="12"/>
     </row>
     <row r="298" ht="20.35" customHeight="1">
       <c r="A298" s="15">
@@ -7584,6 +8071,7 @@
       <c r="F298" s="12"/>
       <c r="G298" s="12"/>
       <c r="H298" s="12"/>
+      <c r="I298" s="12"/>
     </row>
     <row r="299" ht="20.35" customHeight="1">
       <c r="A299" s="15">
@@ -7604,6 +8092,7 @@
       <c r="F299" s="12"/>
       <c r="G299" s="12"/>
       <c r="H299" s="12"/>
+      <c r="I299" s="12"/>
     </row>
     <row r="300" ht="20.35" customHeight="1">
       <c r="A300" s="15">
@@ -7624,6 +8113,7 @@
       <c r="F300" s="12"/>
       <c r="G300" s="12"/>
       <c r="H300" s="12"/>
+      <c r="I300" s="12"/>
     </row>
     <row r="301" ht="20.35" customHeight="1">
       <c r="A301" s="15">
@@ -7644,6 +8134,7 @@
       <c r="F301" s="12"/>
       <c r="G301" s="12"/>
       <c r="H301" s="12"/>
+      <c r="I301" s="12"/>
     </row>
     <row r="302" ht="20.35" customHeight="1">
       <c r="A302" s="10">
@@ -7664,6 +8155,7 @@
       <c r="F302" s="12"/>
       <c r="G302" s="12"/>
       <c r="H302" s="12"/>
+      <c r="I302" s="12"/>
     </row>
     <row r="303" ht="20.35" customHeight="1">
       <c r="A303" s="10">
@@ -7684,6 +8176,7 @@
       <c r="F303" s="12"/>
       <c r="G303" s="12"/>
       <c r="H303" s="12"/>
+      <c r="I303" s="12"/>
     </row>
     <row r="304" ht="20.35" customHeight="1">
       <c r="A304" s="10">
@@ -7704,6 +8197,7 @@
       <c r="F304" s="12"/>
       <c r="G304" s="12"/>
       <c r="H304" s="12"/>
+      <c r="I304" s="12"/>
     </row>
     <row r="305" ht="20.35" customHeight="1">
       <c r="A305" s="10">
@@ -7724,6 +8218,7 @@
       <c r="F305" s="12"/>
       <c r="G305" s="12"/>
       <c r="H305" s="12"/>
+      <c r="I305" s="12"/>
     </row>
     <row r="306" ht="20.35" customHeight="1">
       <c r="A306" s="10">
@@ -7744,6 +8239,7 @@
       <c r="F306" s="12"/>
       <c r="G306" s="12"/>
       <c r="H306" s="12"/>
+      <c r="I306" s="12"/>
     </row>
     <row r="307" ht="20.35" customHeight="1">
       <c r="A307" s="10">
@@ -7764,6 +8260,7 @@
       <c r="F307" s="12"/>
       <c r="G307" s="12"/>
       <c r="H307" s="12"/>
+      <c r="I307" s="12"/>
     </row>
     <row r="308" ht="20.35" customHeight="1">
       <c r="A308" s="10">
@@ -7781,9 +8278,14 @@
       <c r="E308" s="12">
         <v>24</v>
       </c>
-      <c r="F308" s="12"/>
+      <c r="F308" t="s" s="13">
+        <v>61</v>
+      </c>
       <c r="G308" s="12"/>
-      <c r="H308" s="12"/>
+      <c r="H308" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="I308" s="12"/>
     </row>
     <row r="309" ht="20.35" customHeight="1">
       <c r="A309" s="10">
@@ -7804,6 +8306,7 @@
       <c r="F309" s="12"/>
       <c r="G309" s="12"/>
       <c r="H309" s="12"/>
+      <c r="I309" s="12"/>
     </row>
     <row r="310" ht="20.35" customHeight="1">
       <c r="A310" s="10">
@@ -7824,6 +8327,7 @@
       <c r="F310" s="12"/>
       <c r="G310" s="12"/>
       <c r="H310" s="12"/>
+      <c r="I310" s="12"/>
     </row>
     <row r="311" ht="20.35" customHeight="1">
       <c r="A311" s="10">
@@ -7844,6 +8348,7 @@
       <c r="F311" s="12"/>
       <c r="G311" s="12"/>
       <c r="H311" s="12"/>
+      <c r="I311" s="12"/>
     </row>
     <row r="312" ht="20.35" customHeight="1">
       <c r="A312" s="15">
@@ -7864,6 +8369,7 @@
       <c r="F312" s="12"/>
       <c r="G312" s="12"/>
       <c r="H312" s="12"/>
+      <c r="I312" s="12"/>
     </row>
     <row r="313" ht="20.35" customHeight="1">
       <c r="A313" s="15">
@@ -7884,6 +8390,7 @@
       <c r="F313" s="12"/>
       <c r="G313" s="12"/>
       <c r="H313" s="12"/>
+      <c r="I313" s="12"/>
     </row>
     <row r="314" ht="20.35" customHeight="1">
       <c r="A314" s="15">
@@ -7904,6 +8411,7 @@
       <c r="F314" s="12"/>
       <c r="G314" s="12"/>
       <c r="H314" s="12"/>
+      <c r="I314" s="12"/>
     </row>
     <row r="315" ht="20.35" customHeight="1">
       <c r="A315" s="15">
@@ -7924,6 +8432,7 @@
       <c r="F315" s="12"/>
       <c r="G315" s="12"/>
       <c r="H315" s="12"/>
+      <c r="I315" s="12"/>
     </row>
     <row r="316" ht="20.35" customHeight="1">
       <c r="A316" s="15">
@@ -7941,9 +8450,14 @@
       <c r="E316" s="12">
         <v>26</v>
       </c>
-      <c r="F316" s="12"/>
+      <c r="F316" t="s" s="13">
+        <v>62</v>
+      </c>
       <c r="G316" s="12"/>
-      <c r="H316" s="12"/>
+      <c r="H316" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="I316" s="12"/>
     </row>
     <row r="317" ht="20.35" customHeight="1">
       <c r="A317" s="15">
@@ -7964,6 +8478,7 @@
       <c r="F317" s="12"/>
       <c r="G317" s="12"/>
       <c r="H317" s="12"/>
+      <c r="I317" s="12"/>
     </row>
     <row r="318" ht="20.35" customHeight="1">
       <c r="A318" s="15">
@@ -7984,6 +8499,7 @@
       <c r="F318" s="12"/>
       <c r="G318" s="12"/>
       <c r="H318" s="12"/>
+      <c r="I318" s="12"/>
     </row>
     <row r="319" ht="20.35" customHeight="1">
       <c r="A319" s="15">
@@ -8004,6 +8520,7 @@
       <c r="F319" s="12"/>
       <c r="G319" s="12"/>
       <c r="H319" s="12"/>
+      <c r="I319" s="12"/>
     </row>
     <row r="320" ht="20.35" customHeight="1">
       <c r="A320" s="15">
@@ -8024,6 +8541,7 @@
       <c r="F320" s="12"/>
       <c r="G320" s="12"/>
       <c r="H320" s="12"/>
+      <c r="I320" s="12"/>
     </row>
     <row r="321" ht="20.35" customHeight="1">
       <c r="A321" s="15">
@@ -8044,6 +8562,7 @@
       <c r="F321" s="12"/>
       <c r="G321" s="12"/>
       <c r="H321" s="12"/>
+      <c r="I321" s="12"/>
     </row>
     <row r="322" ht="39" customHeight="1">
       <c r="A322" s="10">
@@ -8062,7 +8581,7 @@
         <v>26</v>
       </c>
       <c r="F322" t="s" s="14">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="G322" t="s" s="14">
         <v>18</v>
@@ -8070,6 +8589,7 @@
       <c r="H322" t="s" s="13">
         <v>27</v>
       </c>
+      <c r="I322" s="13"/>
     </row>
     <row r="323" ht="20.35" customHeight="1">
       <c r="A323" s="10">
@@ -8090,6 +8610,7 @@
       <c r="F323" s="12"/>
       <c r="G323" s="12"/>
       <c r="H323" s="12"/>
+      <c r="I323" s="12"/>
     </row>
     <row r="324" ht="20.35" customHeight="1">
       <c r="A324" s="10">
@@ -8110,6 +8631,7 @@
       <c r="F324" s="12"/>
       <c r="G324" s="12"/>
       <c r="H324" s="12"/>
+      <c r="I324" s="12"/>
     </row>
     <row r="325" ht="20.35" customHeight="1">
       <c r="A325" s="10">
@@ -8130,6 +8652,7 @@
       <c r="F325" s="12"/>
       <c r="G325" s="12"/>
       <c r="H325" s="12"/>
+      <c r="I325" s="12"/>
     </row>
     <row r="326" ht="20.35" customHeight="1">
       <c r="A326" s="10">
@@ -8150,6 +8673,7 @@
       <c r="F326" s="12"/>
       <c r="G326" s="12"/>
       <c r="H326" s="12"/>
+      <c r="I326" s="12"/>
     </row>
     <row r="327" ht="20.35" customHeight="1">
       <c r="A327" s="10">
@@ -8170,6 +8694,7 @@
       <c r="F327" s="12"/>
       <c r="G327" s="12"/>
       <c r="H327" s="12"/>
+      <c r="I327" s="12"/>
     </row>
     <row r="328" ht="20.35" customHeight="1">
       <c r="A328" s="10">
@@ -8190,6 +8715,7 @@
       <c r="F328" s="12"/>
       <c r="G328" s="12"/>
       <c r="H328" s="12"/>
+      <c r="I328" s="12"/>
     </row>
     <row r="329" ht="20.35" customHeight="1">
       <c r="A329" s="10">
@@ -8210,6 +8736,7 @@
       <c r="F329" s="12"/>
       <c r="G329" s="12"/>
       <c r="H329" s="12"/>
+      <c r="I329" s="12"/>
     </row>
     <row r="330" ht="20.35" customHeight="1">
       <c r="A330" s="10">
@@ -8230,6 +8757,7 @@
       <c r="F330" s="12"/>
       <c r="G330" s="12"/>
       <c r="H330" s="12"/>
+      <c r="I330" s="12"/>
     </row>
     <row r="331" ht="20.35" customHeight="1">
       <c r="A331" s="10">
@@ -8250,6 +8778,7 @@
       <c r="F331" s="12"/>
       <c r="G331" s="12"/>
       <c r="H331" s="12"/>
+      <c r="I331" s="12"/>
     </row>
     <row r="332" ht="20.35" customHeight="1">
       <c r="A332" s="15">
@@ -8270,6 +8799,7 @@
       <c r="F332" s="12"/>
       <c r="G332" s="12"/>
       <c r="H332" s="12"/>
+      <c r="I332" s="12"/>
     </row>
     <row r="333" ht="20.35" customHeight="1">
       <c r="A333" s="15">
@@ -8290,6 +8820,7 @@
       <c r="F333" s="12"/>
       <c r="G333" s="12"/>
       <c r="H333" s="12"/>
+      <c r="I333" s="12"/>
     </row>
     <row r="334" ht="20.35" customHeight="1">
       <c r="A334" s="15">
@@ -8310,6 +8841,7 @@
       <c r="F334" s="12"/>
       <c r="G334" s="12"/>
       <c r="H334" s="12"/>
+      <c r="I334" s="12"/>
     </row>
     <row r="335" ht="20.35" customHeight="1">
       <c r="A335" s="15">
@@ -8330,6 +8862,7 @@
       <c r="F335" s="12"/>
       <c r="G335" s="12"/>
       <c r="H335" s="12"/>
+      <c r="I335" s="12"/>
     </row>
     <row r="336" ht="20.35" customHeight="1">
       <c r="A336" s="15">
@@ -8350,6 +8883,7 @@
       <c r="F336" s="12"/>
       <c r="G336" s="12"/>
       <c r="H336" s="12"/>
+      <c r="I336" s="12"/>
     </row>
     <row r="337" ht="20.35" customHeight="1">
       <c r="A337" s="15">
@@ -8367,9 +8901,14 @@
       <c r="E337" s="12">
         <v>29</v>
       </c>
-      <c r="F337" s="12"/>
-      <c r="G337" s="12"/>
-      <c r="H337" s="12"/>
+      <c r="F337" t="s" s="13">
+        <v>64</v>
+      </c>
+      <c r="G337" s="22"/>
+      <c r="H337" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="I337" s="12"/>
     </row>
     <row r="338" ht="20.35" customHeight="1">
       <c r="A338" s="15">
@@ -8390,6 +8929,7 @@
       <c r="F338" s="12"/>
       <c r="G338" s="12"/>
       <c r="H338" s="12"/>
+      <c r="I338" s="12"/>
     </row>
     <row r="339" ht="20.35" customHeight="1">
       <c r="A339" s="15">
@@ -8410,6 +8950,7 @@
       <c r="F339" s="12"/>
       <c r="G339" s="12"/>
       <c r="H339" s="12"/>
+      <c r="I339" s="12"/>
     </row>
     <row r="340" ht="20.35" customHeight="1">
       <c r="A340" s="15">
@@ -8430,6 +8971,7 @@
       <c r="F340" s="12"/>
       <c r="G340" s="12"/>
       <c r="H340" s="12"/>
+      <c r="I340" s="12"/>
     </row>
     <row r="341" ht="20.35" customHeight="1">
       <c r="A341" s="15">
@@ -8450,6 +8992,7 @@
       <c r="F341" s="12"/>
       <c r="G341" s="12"/>
       <c r="H341" s="12"/>
+      <c r="I341" s="12"/>
     </row>
     <row r="342" ht="20.35" customHeight="1">
       <c r="A342" s="10">
@@ -8470,6 +9013,7 @@
       <c r="F342" s="12"/>
       <c r="G342" s="12"/>
       <c r="H342" s="12"/>
+      <c r="I342" s="12"/>
     </row>
     <row r="343" ht="20.35" customHeight="1">
       <c r="A343" s="10">
@@ -8490,6 +9034,7 @@
       <c r="F343" s="12"/>
       <c r="G343" s="12"/>
       <c r="H343" s="12"/>
+      <c r="I343" s="12"/>
     </row>
     <row r="344" ht="20.35" customHeight="1">
       <c r="A344" s="10">
@@ -8510,6 +9055,7 @@
       <c r="F344" s="12"/>
       <c r="G344" s="12"/>
       <c r="H344" s="12"/>
+      <c r="I344" s="12"/>
     </row>
     <row r="345" ht="20.35" customHeight="1">
       <c r="A345" s="10">
@@ -8530,6 +9076,7 @@
       <c r="F345" s="12"/>
       <c r="G345" s="12"/>
       <c r="H345" s="12"/>
+      <c r="I345" s="12"/>
     </row>
     <row r="346" ht="20.35" customHeight="1">
       <c r="A346" s="10">
@@ -8550,6 +9097,7 @@
       <c r="F346" s="12"/>
       <c r="G346" s="12"/>
       <c r="H346" s="12"/>
+      <c r="I346" s="12"/>
     </row>
     <row r="347" ht="20.35" customHeight="1">
       <c r="A347" s="10">
@@ -8570,6 +9118,7 @@
       <c r="F347" s="12"/>
       <c r="G347" s="12"/>
       <c r="H347" s="12"/>
+      <c r="I347" s="12"/>
     </row>
     <row r="348" ht="20.35" customHeight="1">
       <c r="A348" s="10">
@@ -8590,6 +9139,7 @@
       <c r="F348" s="12"/>
       <c r="G348" s="12"/>
       <c r="H348" s="12"/>
+      <c r="I348" s="12"/>
     </row>
     <row r="349" ht="20.35" customHeight="1">
       <c r="A349" s="10">
@@ -8610,6 +9160,7 @@
       <c r="F349" s="12"/>
       <c r="G349" s="12"/>
       <c r="H349" s="12"/>
+      <c r="I349" s="12"/>
     </row>
     <row r="350" ht="20.35" customHeight="1">
       <c r="A350" s="10">
@@ -8630,6 +9181,7 @@
       <c r="F350" s="12"/>
       <c r="G350" s="12"/>
       <c r="H350" s="12"/>
+      <c r="I350" s="12"/>
     </row>
     <row r="351" ht="20.35" customHeight="1">
       <c r="A351" s="10">
@@ -8650,6 +9202,7 @@
       <c r="F351" s="12"/>
       <c r="G351" s="12"/>
       <c r="H351" s="12"/>
+      <c r="I351" s="12"/>
     </row>
     <row r="352" ht="20.35" customHeight="1">
       <c r="A352" s="15">
@@ -8670,6 +9223,7 @@
       <c r="F352" s="12"/>
       <c r="G352" s="12"/>
       <c r="H352" s="12"/>
+      <c r="I352" s="12"/>
     </row>
     <row r="353" ht="20.35" customHeight="1">
       <c r="A353" s="15">
@@ -8690,6 +9244,7 @@
       <c r="F353" s="12"/>
       <c r="G353" s="12"/>
       <c r="H353" s="12"/>
+      <c r="I353" s="12"/>
     </row>
     <row r="354" ht="20.35" customHeight="1">
       <c r="A354" s="15">
@@ -8710,6 +9265,7 @@
       <c r="F354" s="12"/>
       <c r="G354" s="12"/>
       <c r="H354" s="12"/>
+      <c r="I354" s="12"/>
     </row>
     <row r="355" ht="20.35" customHeight="1">
       <c r="A355" s="15">
@@ -8730,6 +9286,7 @@
       <c r="F355" s="12"/>
       <c r="G355" s="12"/>
       <c r="H355" s="12"/>
+      <c r="I355" s="12"/>
     </row>
     <row r="356" ht="20.35" customHeight="1">
       <c r="A356" s="15">
@@ -8750,6 +9307,7 @@
       <c r="F356" s="12"/>
       <c r="G356" s="12"/>
       <c r="H356" s="12"/>
+      <c r="I356" s="12"/>
     </row>
     <row r="357" ht="20.35" customHeight="1">
       <c r="A357" s="15">
@@ -8770,6 +9328,7 @@
       <c r="F357" s="12"/>
       <c r="G357" s="12"/>
       <c r="H357" s="12"/>
+      <c r="I357" s="12"/>
     </row>
     <row r="358" ht="20.35" customHeight="1">
       <c r="A358" s="15">
@@ -8790,6 +9349,7 @@
       <c r="F358" s="12"/>
       <c r="G358" s="12"/>
       <c r="H358" s="12"/>
+      <c r="I358" s="12"/>
     </row>
     <row r="359" ht="20.35" customHeight="1">
       <c r="A359" s="15">
@@ -8810,6 +9370,7 @@
       <c r="F359" s="12"/>
       <c r="G359" s="12"/>
       <c r="H359" s="12"/>
+      <c r="I359" s="12"/>
     </row>
     <row r="360" ht="20.35" customHeight="1">
       <c r="A360" s="15">
@@ -8830,6 +9391,7 @@
       <c r="F360" s="12"/>
       <c r="G360" s="12"/>
       <c r="H360" s="12"/>
+      <c r="I360" s="12"/>
     </row>
     <row r="361" ht="20.35" customHeight="1">
       <c r="A361" s="15">
@@ -8850,6 +9412,7 @@
       <c r="F361" s="12"/>
       <c r="G361" s="12"/>
       <c r="H361" s="12"/>
+      <c r="I361" s="12"/>
     </row>
     <row r="362" ht="20.35" customHeight="1">
       <c r="A362" s="10">
@@ -8870,6 +9433,7 @@
       <c r="F362" s="12"/>
       <c r="G362" s="12"/>
       <c r="H362" s="12"/>
+      <c r="I362" s="12"/>
     </row>
     <row r="363" ht="20.35" customHeight="1">
       <c r="A363" s="10">
@@ -8890,6 +9454,7 @@
       <c r="F363" s="12"/>
       <c r="G363" s="12"/>
       <c r="H363" s="12"/>
+      <c r="I363" s="12"/>
     </row>
     <row r="364" ht="20.35" customHeight="1">
       <c r="A364" s="10">
@@ -8910,6 +9475,7 @@
       <c r="F364" s="12"/>
       <c r="G364" s="12"/>
       <c r="H364" s="12"/>
+      <c r="I364" s="12"/>
     </row>
     <row r="365" ht="20.35" customHeight="1">
       <c r="A365" s="10">
@@ -8930,6 +9496,7 @@
       <c r="F365" s="12"/>
       <c r="G365" s="12"/>
       <c r="H365" s="12"/>
+      <c r="I365" s="12"/>
     </row>
     <row r="366" ht="20.35" customHeight="1">
       <c r="A366" s="10">
@@ -8950,6 +9517,7 @@
       <c r="F366" s="12"/>
       <c r="G366" s="12"/>
       <c r="H366" s="12"/>
+      <c r="I366" s="12"/>
     </row>
     <row r="367" ht="20.35" customHeight="1">
       <c r="A367" s="10">
@@ -8970,6 +9538,7 @@
       <c r="F367" s="12"/>
       <c r="G367" s="12"/>
       <c r="H367" s="12"/>
+      <c r="I367" s="12"/>
     </row>
     <row r="368" ht="20.35" customHeight="1">
       <c r="A368" s="10">
@@ -8990,6 +9559,7 @@
       <c r="F368" s="12"/>
       <c r="G368" s="12"/>
       <c r="H368" s="12"/>
+      <c r="I368" s="12"/>
     </row>
     <row r="369" ht="20.35" customHeight="1">
       <c r="A369" s="10">
@@ -9010,6 +9580,7 @@
       <c r="F369" s="12"/>
       <c r="G369" s="12"/>
       <c r="H369" s="12"/>
+      <c r="I369" s="12"/>
     </row>
     <row r="370" ht="20.35" customHeight="1">
       <c r="A370" s="10">
@@ -9030,6 +9601,7 @@
       <c r="F370" s="12"/>
       <c r="G370" s="12"/>
       <c r="H370" s="12"/>
+      <c r="I370" s="12"/>
     </row>
     <row r="371" ht="20.35" customHeight="1">
       <c r="A371" s="10">
@@ -9050,6 +9622,7 @@
       <c r="F371" s="12"/>
       <c r="G371" s="12"/>
       <c r="H371" s="12"/>
+      <c r="I371" s="12"/>
     </row>
     <row r="372" ht="20.35" customHeight="1">
       <c r="A372" s="15">
@@ -9070,6 +9643,7 @@
       <c r="F372" s="12"/>
       <c r="G372" s="12"/>
       <c r="H372" s="12"/>
+      <c r="I372" s="12"/>
     </row>
     <row r="373" ht="20.35" customHeight="1">
       <c r="A373" s="15">
@@ -9090,6 +9664,7 @@
       <c r="F373" s="12"/>
       <c r="G373" s="12"/>
       <c r="H373" s="12"/>
+      <c r="I373" s="12"/>
     </row>
     <row r="374" ht="20.35" customHeight="1">
       <c r="A374" s="15">
@@ -9110,6 +9685,7 @@
       <c r="F374" s="12"/>
       <c r="G374" s="12"/>
       <c r="H374" s="12"/>
+      <c r="I374" s="12"/>
     </row>
     <row r="375" ht="20.35" customHeight="1">
       <c r="A375" s="15">
@@ -9130,6 +9706,7 @@
       <c r="F375" s="12"/>
       <c r="G375" s="12"/>
       <c r="H375" s="12"/>
+      <c r="I375" s="12"/>
     </row>
     <row r="376" ht="20.35" customHeight="1">
       <c r="A376" s="15">
@@ -9150,6 +9727,7 @@
       <c r="F376" s="12"/>
       <c r="G376" s="12"/>
       <c r="H376" s="12"/>
+      <c r="I376" s="12"/>
     </row>
     <row r="377" ht="20.35" customHeight="1">
       <c r="A377" s="15">
@@ -9170,6 +9748,7 @@
       <c r="F377" s="12"/>
       <c r="G377" s="12"/>
       <c r="H377" s="12"/>
+      <c r="I377" s="12"/>
     </row>
     <row r="378" ht="20.35" customHeight="1">
       <c r="A378" s="15">
@@ -9190,6 +9769,7 @@
       <c r="F378" s="12"/>
       <c r="G378" s="12"/>
       <c r="H378" s="12"/>
+      <c r="I378" s="12"/>
     </row>
     <row r="379" ht="20.35" customHeight="1">
       <c r="A379" s="15">
@@ -9210,6 +9790,7 @@
       <c r="F379" s="12"/>
       <c r="G379" s="12"/>
       <c r="H379" s="12"/>
+      <c r="I379" s="12"/>
     </row>
     <row r="380" ht="20.35" customHeight="1">
       <c r="A380" s="15">
@@ -9230,6 +9811,7 @@
       <c r="F380" s="12"/>
       <c r="G380" s="12"/>
       <c r="H380" s="12"/>
+      <c r="I380" s="12"/>
     </row>
     <row r="381" ht="20.35" customHeight="1">
       <c r="A381" s="15">
@@ -9250,6 +9832,7 @@
       <c r="F381" s="12"/>
       <c r="G381" s="12"/>
       <c r="H381" s="12"/>
+      <c r="I381" s="12"/>
     </row>
     <row r="382" ht="20.35" customHeight="1">
       <c r="A382" s="10">
@@ -9270,6 +9853,7 @@
       <c r="F382" s="12"/>
       <c r="G382" s="12"/>
       <c r="H382" s="12"/>
+      <c r="I382" s="12"/>
     </row>
     <row r="383" ht="20.35" customHeight="1">
       <c r="A383" s="10">
@@ -9290,6 +9874,7 @@
       <c r="F383" s="12"/>
       <c r="G383" s="12"/>
       <c r="H383" s="12"/>
+      <c r="I383" s="12"/>
     </row>
     <row r="384" ht="20.35" customHeight="1">
       <c r="A384" s="10">
@@ -9310,6 +9895,7 @@
       <c r="F384" s="12"/>
       <c r="G384" s="12"/>
       <c r="H384" s="12"/>
+      <c r="I384" s="12"/>
     </row>
     <row r="385" ht="20.35" customHeight="1">
       <c r="A385" s="10">
@@ -9330,6 +9916,7 @@
       <c r="F385" s="12"/>
       <c r="G385" s="12"/>
       <c r="H385" s="12"/>
+      <c r="I385" s="12"/>
     </row>
     <row r="386" ht="20.35" customHeight="1">
       <c r="A386" s="10">
@@ -9350,6 +9937,7 @@
       <c r="F386" s="12"/>
       <c r="G386" s="12"/>
       <c r="H386" s="12"/>
+      <c r="I386" s="12"/>
     </row>
     <row r="387" ht="20.35" customHeight="1">
       <c r="A387" s="10">
@@ -9370,6 +9958,7 @@
       <c r="F387" s="12"/>
       <c r="G387" s="12"/>
       <c r="H387" s="12"/>
+      <c r="I387" s="12"/>
     </row>
     <row r="388" ht="20.35" customHeight="1">
       <c r="A388" s="10">
@@ -9390,6 +9979,7 @@
       <c r="F388" s="12"/>
       <c r="G388" s="12"/>
       <c r="H388" s="12"/>
+      <c r="I388" s="12"/>
     </row>
     <row r="389" ht="20.35" customHeight="1">
       <c r="A389" s="10">
@@ -9410,6 +10000,7 @@
       <c r="F389" s="12"/>
       <c r="G389" s="12"/>
       <c r="H389" s="12"/>
+      <c r="I389" s="12"/>
     </row>
     <row r="390" ht="20.35" customHeight="1">
       <c r="A390" s="10">
@@ -9430,6 +10021,7 @@
       <c r="F390" s="12"/>
       <c r="G390" s="12"/>
       <c r="H390" s="12"/>
+      <c r="I390" s="12"/>
     </row>
     <row r="391" ht="20.35" customHeight="1">
       <c r="A391" s="10">
@@ -9450,6 +10042,7 @@
       <c r="F391" s="12"/>
       <c r="G391" s="12"/>
       <c r="H391" s="12"/>
+      <c r="I391" s="12"/>
     </row>
     <row r="392" ht="20.35" customHeight="1">
       <c r="A392" s="15">
@@ -9470,6 +10063,7 @@
       <c r="F392" s="12"/>
       <c r="G392" s="12"/>
       <c r="H392" s="12"/>
+      <c r="I392" s="12"/>
     </row>
     <row r="393" ht="20.35" customHeight="1">
       <c r="A393" s="15">
@@ -9490,6 +10084,7 @@
       <c r="F393" s="12"/>
       <c r="G393" s="12"/>
       <c r="H393" s="12"/>
+      <c r="I393" s="12"/>
     </row>
     <row r="394" ht="20.35" customHeight="1">
       <c r="A394" s="15">
@@ -9510,6 +10105,7 @@
       <c r="F394" s="12"/>
       <c r="G394" s="12"/>
       <c r="H394" s="12"/>
+      <c r="I394" s="12"/>
     </row>
     <row r="395" ht="20.35" customHeight="1">
       <c r="A395" s="15">
@@ -9530,6 +10126,7 @@
       <c r="F395" s="12"/>
       <c r="G395" s="12"/>
       <c r="H395" s="12"/>
+      <c r="I395" s="12"/>
     </row>
     <row r="396" ht="20.35" customHeight="1">
       <c r="A396" s="15">
@@ -9550,6 +10147,7 @@
       <c r="F396" s="12"/>
       <c r="G396" s="12"/>
       <c r="H396" s="12"/>
+      <c r="I396" s="12"/>
     </row>
     <row r="397" ht="20.35" customHeight="1">
       <c r="A397" s="15">
@@ -9570,6 +10168,7 @@
       <c r="F397" s="12"/>
       <c r="G397" s="12"/>
       <c r="H397" s="12"/>
+      <c r="I397" s="12"/>
     </row>
     <row r="398" ht="20.35" customHeight="1">
       <c r="A398" s="15">
@@ -9590,6 +10189,7 @@
       <c r="F398" s="12"/>
       <c r="G398" s="12"/>
       <c r="H398" s="12"/>
+      <c r="I398" s="12"/>
     </row>
     <row r="399" ht="20.35" customHeight="1">
       <c r="A399" s="15">
@@ -9610,6 +10210,7 @@
       <c r="F399" s="12"/>
       <c r="G399" s="12"/>
       <c r="H399" s="12"/>
+      <c r="I399" s="12"/>
     </row>
     <row r="400" ht="20.35" customHeight="1">
       <c r="A400" s="15">
@@ -9630,6 +10231,7 @@
       <c r="F400" s="12"/>
       <c r="G400" s="12"/>
       <c r="H400" s="12"/>
+      <c r="I400" s="12"/>
     </row>
     <row r="401" ht="20.35" customHeight="1">
       <c r="A401" s="15">
@@ -9650,6 +10252,7 @@
       <c r="F401" s="12"/>
       <c r="G401" s="12"/>
       <c r="H401" s="12"/>
+      <c r="I401" s="12"/>
     </row>
     <row r="402" ht="20.35" customHeight="1">
       <c r="A402" s="10">
@@ -9670,6 +10273,7 @@
       <c r="F402" s="12"/>
       <c r="G402" s="12"/>
       <c r="H402" s="12"/>
+      <c r="I402" s="12"/>
     </row>
     <row r="403" ht="20.35" customHeight="1">
       <c r="A403" s="10">
@@ -9690,6 +10294,7 @@
       <c r="F403" s="12"/>
       <c r="G403" s="12"/>
       <c r="H403" s="12"/>
+      <c r="I403" s="12"/>
     </row>
     <row r="404" ht="20.35" customHeight="1">
       <c r="A404" s="10">
@@ -9710,6 +10315,7 @@
       <c r="F404" s="12"/>
       <c r="G404" s="12"/>
       <c r="H404" s="12"/>
+      <c r="I404" s="12"/>
     </row>
     <row r="405" ht="20.35" customHeight="1">
       <c r="A405" s="10">
@@ -9730,6 +10336,7 @@
       <c r="F405" s="12"/>
       <c r="G405" s="12"/>
       <c r="H405" s="12"/>
+      <c r="I405" s="12"/>
     </row>
     <row r="406" ht="20.35" customHeight="1">
       <c r="A406" s="10">
@@ -9750,6 +10357,7 @@
       <c r="F406" s="12"/>
       <c r="G406" s="12"/>
       <c r="H406" s="12"/>
+      <c r="I406" s="12"/>
     </row>
     <row r="407" ht="20.35" customHeight="1">
       <c r="A407" s="10">
@@ -9770,6 +10378,7 @@
       <c r="F407" s="12"/>
       <c r="G407" s="12"/>
       <c r="H407" s="12"/>
+      <c r="I407" s="12"/>
     </row>
     <row r="408" ht="20.35" customHeight="1">
       <c r="A408" s="10">
@@ -9790,6 +10399,7 @@
       <c r="F408" s="12"/>
       <c r="G408" s="12"/>
       <c r="H408" s="12"/>
+      <c r="I408" s="12"/>
     </row>
     <row r="409" ht="20.35" customHeight="1">
       <c r="A409" s="10">
@@ -9810,6 +10420,7 @@
       <c r="F409" s="12"/>
       <c r="G409" s="12"/>
       <c r="H409" s="12"/>
+      <c r="I409" s="12"/>
     </row>
     <row r="410" ht="20.35" customHeight="1">
       <c r="A410" s="10">
@@ -9830,6 +10441,7 @@
       <c r="F410" s="12"/>
       <c r="G410" s="12"/>
       <c r="H410" s="12"/>
+      <c r="I410" s="12"/>
     </row>
     <row r="411" ht="20.35" customHeight="1">
       <c r="A411" s="10">
@@ -9850,6 +10462,7 @@
       <c r="F411" s="12"/>
       <c r="G411" s="12"/>
       <c r="H411" s="12"/>
+      <c r="I411" s="12"/>
     </row>
     <row r="412" ht="20.35" customHeight="1">
       <c r="A412" s="15">
@@ -9870,6 +10483,7 @@
       <c r="F412" s="12"/>
       <c r="G412" s="12"/>
       <c r="H412" s="12"/>
+      <c r="I412" s="12"/>
     </row>
     <row r="413" ht="20.35" customHeight="1">
       <c r="A413" s="15">
@@ -9890,6 +10504,7 @@
       <c r="F413" s="12"/>
       <c r="G413" s="12"/>
       <c r="H413" s="12"/>
+      <c r="I413" s="12"/>
     </row>
     <row r="414" ht="20.35" customHeight="1">
       <c r="A414" s="15">
@@ -9910,6 +10525,7 @@
       <c r="F414" s="12"/>
       <c r="G414" s="12"/>
       <c r="H414" s="12"/>
+      <c r="I414" s="12"/>
     </row>
     <row r="415" ht="20.35" customHeight="1">
       <c r="A415" s="15">
@@ -9930,6 +10546,7 @@
       <c r="F415" s="12"/>
       <c r="G415" s="12"/>
       <c r="H415" s="12"/>
+      <c r="I415" s="12"/>
     </row>
     <row r="416" ht="20.35" customHeight="1">
       <c r="A416" s="15">
@@ -9950,6 +10567,7 @@
       <c r="F416" s="12"/>
       <c r="G416" s="12"/>
       <c r="H416" s="12"/>
+      <c r="I416" s="12"/>
     </row>
     <row r="417" ht="20.35" customHeight="1">
       <c r="A417" s="15">
@@ -9970,6 +10588,7 @@
       <c r="F417" s="12"/>
       <c r="G417" s="12"/>
       <c r="H417" s="12"/>
+      <c r="I417" s="12"/>
     </row>
     <row r="418" ht="20.35" customHeight="1">
       <c r="A418" s="15">
@@ -9990,6 +10609,7 @@
       <c r="F418" s="12"/>
       <c r="G418" s="12"/>
       <c r="H418" s="12"/>
+      <c r="I418" s="12"/>
     </row>
     <row r="419" ht="20.35" customHeight="1">
       <c r="A419" s="15">
@@ -10010,6 +10630,7 @@
       <c r="F419" s="12"/>
       <c r="G419" s="12"/>
       <c r="H419" s="12"/>
+      <c r="I419" s="12"/>
     </row>
     <row r="420" ht="20.35" customHeight="1">
       <c r="A420" s="15">
@@ -10030,6 +10651,7 @@
       <c r="F420" s="12"/>
       <c r="G420" s="12"/>
       <c r="H420" s="12"/>
+      <c r="I420" s="12"/>
     </row>
     <row r="421" ht="20.35" customHeight="1">
       <c r="A421" s="15">
@@ -10050,6 +10672,7 @@
       <c r="F421" s="12"/>
       <c r="G421" s="12"/>
       <c r="H421" s="12"/>
+      <c r="I421" s="12"/>
     </row>
     <row r="422" ht="20.35" customHeight="1">
       <c r="A422" s="10">
@@ -10070,6 +10693,7 @@
       <c r="F422" s="12"/>
       <c r="G422" s="12"/>
       <c r="H422" s="12"/>
+      <c r="I422" s="12"/>
     </row>
     <row r="423" ht="20.35" customHeight="1">
       <c r="A423" s="10">
@@ -10090,6 +10714,7 @@
       <c r="F423" s="12"/>
       <c r="G423" s="12"/>
       <c r="H423" s="12"/>
+      <c r="I423" s="12"/>
     </row>
     <row r="424" ht="20.35" customHeight="1">
       <c r="A424" s="10">
@@ -10110,6 +10735,7 @@
       <c r="F424" s="12"/>
       <c r="G424" s="12"/>
       <c r="H424" s="12"/>
+      <c r="I424" s="12"/>
     </row>
     <row r="425" ht="20.35" customHeight="1">
       <c r="A425" s="10">
@@ -10130,6 +10756,7 @@
       <c r="F425" s="12"/>
       <c r="G425" s="12"/>
       <c r="H425" s="12"/>
+      <c r="I425" s="12"/>
     </row>
     <row r="426" ht="20.35" customHeight="1">
       <c r="A426" s="10">
@@ -10150,6 +10777,7 @@
       <c r="F426" s="12"/>
       <c r="G426" s="12"/>
       <c r="H426" s="12"/>
+      <c r="I426" s="12"/>
     </row>
     <row r="427" ht="20.35" customHeight="1">
       <c r="A427" s="10">
@@ -10170,6 +10798,7 @@
       <c r="F427" s="12"/>
       <c r="G427" s="12"/>
       <c r="H427" s="12"/>
+      <c r="I427" s="12"/>
     </row>
     <row r="428" ht="20.35" customHeight="1">
       <c r="A428" s="10">
@@ -10190,6 +10819,7 @@
       <c r="F428" s="12"/>
       <c r="G428" s="12"/>
       <c r="H428" s="12"/>
+      <c r="I428" s="12"/>
     </row>
     <row r="429" ht="20.35" customHeight="1">
       <c r="A429" s="10">
@@ -10210,6 +10840,7 @@
       <c r="F429" s="12"/>
       <c r="G429" s="12"/>
       <c r="H429" s="12"/>
+      <c r="I429" s="12"/>
     </row>
     <row r="430" ht="20.35" customHeight="1">
       <c r="A430" s="10">
@@ -10230,6 +10861,7 @@
       <c r="F430" s="12"/>
       <c r="G430" s="12"/>
       <c r="H430" s="12"/>
+      <c r="I430" s="12"/>
     </row>
     <row r="431" ht="20.35" customHeight="1">
       <c r="A431" s="10">
@@ -10250,6 +10882,7 @@
       <c r="F431" s="12"/>
       <c r="G431" s="12"/>
       <c r="H431" s="12"/>
+      <c r="I431" s="12"/>
     </row>
     <row r="432" ht="20.35" customHeight="1">
       <c r="A432" s="15">
@@ -10270,6 +10903,7 @@
       <c r="F432" s="12"/>
       <c r="G432" s="12"/>
       <c r="H432" s="12"/>
+      <c r="I432" s="12"/>
     </row>
     <row r="433" ht="20.35" customHeight="1">
       <c r="A433" s="15">
@@ -10290,6 +10924,7 @@
       <c r="F433" s="12"/>
       <c r="G433" s="12"/>
       <c r="H433" s="12"/>
+      <c r="I433" s="12"/>
     </row>
     <row r="434" ht="20.35" customHeight="1">
       <c r="A434" s="15">
@@ -10310,6 +10945,7 @@
       <c r="F434" s="12"/>
       <c r="G434" s="12"/>
       <c r="H434" s="12"/>
+      <c r="I434" s="12"/>
     </row>
     <row r="435" ht="20.35" customHeight="1">
       <c r="A435" s="15">
@@ -10330,6 +10966,7 @@
       <c r="F435" s="12"/>
       <c r="G435" s="12"/>
       <c r="H435" s="12"/>
+      <c r="I435" s="12"/>
     </row>
     <row r="436" ht="20.35" customHeight="1">
       <c r="A436" s="15">
@@ -10350,6 +10987,7 @@
       <c r="F436" s="12"/>
       <c r="G436" s="12"/>
       <c r="H436" s="12"/>
+      <c r="I436" s="12"/>
     </row>
     <row r="437" ht="20.35" customHeight="1">
       <c r="A437" s="15">
@@ -10370,6 +11008,7 @@
       <c r="F437" s="12"/>
       <c r="G437" s="12"/>
       <c r="H437" s="12"/>
+      <c r="I437" s="12"/>
     </row>
     <row r="438" ht="20.35" customHeight="1">
       <c r="A438" s="15">
@@ -10390,6 +11029,7 @@
       <c r="F438" s="12"/>
       <c r="G438" s="12"/>
       <c r="H438" s="12"/>
+      <c r="I438" s="12"/>
     </row>
     <row r="439" ht="20.35" customHeight="1">
       <c r="A439" s="15">
@@ -10410,6 +11050,7 @@
       <c r="F439" s="12"/>
       <c r="G439" s="12"/>
       <c r="H439" s="12"/>
+      <c r="I439" s="12"/>
     </row>
     <row r="440" ht="20.35" customHeight="1">
       <c r="A440" s="15">
@@ -10430,6 +11071,7 @@
       <c r="F440" s="12"/>
       <c r="G440" s="12"/>
       <c r="H440" s="12"/>
+      <c r="I440" s="12"/>
     </row>
     <row r="441" ht="20.35" customHeight="1">
       <c r="A441" s="15">
@@ -10450,6 +11092,7 @@
       <c r="F441" s="12"/>
       <c r="G441" s="12"/>
       <c r="H441" s="12"/>
+      <c r="I441" s="12"/>
     </row>
     <row r="442" ht="20.35" customHeight="1">
       <c r="A442" s="10">
@@ -10470,6 +11113,7 @@
       <c r="F442" s="12"/>
       <c r="G442" s="12"/>
       <c r="H442" s="12"/>
+      <c r="I442" s="12"/>
     </row>
     <row r="443" ht="20.35" customHeight="1">
       <c r="A443" s="10">
@@ -10490,6 +11134,7 @@
       <c r="F443" s="12"/>
       <c r="G443" s="12"/>
       <c r="H443" s="12"/>
+      <c r="I443" s="12"/>
     </row>
     <row r="444" ht="20.35" customHeight="1">
       <c r="A444" s="10">
@@ -10510,6 +11155,7 @@
       <c r="F444" s="12"/>
       <c r="G444" s="12"/>
       <c r="H444" s="12"/>
+      <c r="I444" s="12"/>
     </row>
     <row r="445" ht="20.35" customHeight="1">
       <c r="A445" s="10">
@@ -10530,6 +11176,7 @@
       <c r="F445" s="12"/>
       <c r="G445" s="12"/>
       <c r="H445" s="12"/>
+      <c r="I445" s="12"/>
     </row>
     <row r="446" ht="20.35" customHeight="1">
       <c r="A446" s="10">
@@ -10550,6 +11197,7 @@
       <c r="F446" s="12"/>
       <c r="G446" s="12"/>
       <c r="H446" s="12"/>
+      <c r="I446" s="12"/>
     </row>
     <row r="447" ht="20.35" customHeight="1">
       <c r="A447" s="10">
@@ -10570,6 +11218,7 @@
       <c r="F447" s="12"/>
       <c r="G447" s="12"/>
       <c r="H447" s="12"/>
+      <c r="I447" s="12"/>
     </row>
     <row r="448" ht="20.35" customHeight="1">
       <c r="A448" s="10">
@@ -10590,6 +11239,7 @@
       <c r="F448" s="12"/>
       <c r="G448" s="12"/>
       <c r="H448" s="12"/>
+      <c r="I448" s="12"/>
     </row>
     <row r="449" ht="20.35" customHeight="1">
       <c r="A449" s="10">
@@ -10610,6 +11260,7 @@
       <c r="F449" s="12"/>
       <c r="G449" s="12"/>
       <c r="H449" s="12"/>
+      <c r="I449" s="12"/>
     </row>
     <row r="450" ht="20.35" customHeight="1">
       <c r="A450" s="10">
@@ -10630,6 +11281,7 @@
       <c r="F450" s="12"/>
       <c r="G450" s="12"/>
       <c r="H450" s="12"/>
+      <c r="I450" s="12"/>
     </row>
     <row r="451" ht="20.35" customHeight="1">
       <c r="A451" s="10">
@@ -10650,6 +11302,7 @@
       <c r="F451" s="12"/>
       <c r="G451" s="12"/>
       <c r="H451" s="12"/>
+      <c r="I451" s="12"/>
     </row>
     <row r="452" ht="20.35" customHeight="1">
       <c r="A452" s="15">
@@ -10670,6 +11323,7 @@
       <c r="F452" s="12"/>
       <c r="G452" s="12"/>
       <c r="H452" s="12"/>
+      <c r="I452" s="12"/>
     </row>
     <row r="453" ht="20.35" customHeight="1">
       <c r="A453" s="15">
@@ -10690,6 +11344,7 @@
       <c r="F453" s="12"/>
       <c r="G453" s="12"/>
       <c r="H453" s="12"/>
+      <c r="I453" s="12"/>
     </row>
     <row r="454" ht="20.35" customHeight="1">
       <c r="A454" s="15">
@@ -10710,6 +11365,7 @@
       <c r="F454" s="12"/>
       <c r="G454" s="12"/>
       <c r="H454" s="12"/>
+      <c r="I454" s="12"/>
     </row>
     <row r="455" ht="20.35" customHeight="1">
       <c r="A455" s="15">
@@ -10730,6 +11386,7 @@
       <c r="F455" s="12"/>
       <c r="G455" s="12"/>
       <c r="H455" s="12"/>
+      <c r="I455" s="12"/>
     </row>
     <row r="456" ht="20.35" customHeight="1">
       <c r="A456" s="15">
@@ -10750,6 +11407,7 @@
       <c r="F456" s="12"/>
       <c r="G456" s="12"/>
       <c r="H456" s="12"/>
+      <c r="I456" s="12"/>
     </row>
     <row r="457" ht="20.35" customHeight="1">
       <c r="A457" s="15">
@@ -10770,6 +11428,7 @@
       <c r="F457" s="12"/>
       <c r="G457" s="12"/>
       <c r="H457" s="12"/>
+      <c r="I457" s="12"/>
     </row>
     <row r="458" ht="20.35" customHeight="1">
       <c r="A458" s="15">
@@ -10790,6 +11449,7 @@
       <c r="F458" s="12"/>
       <c r="G458" s="12"/>
       <c r="H458" s="12"/>
+      <c r="I458" s="12"/>
     </row>
     <row r="459" ht="20.35" customHeight="1">
       <c r="A459" s="15">
@@ -10810,6 +11470,7 @@
       <c r="F459" s="12"/>
       <c r="G459" s="12"/>
       <c r="H459" s="12"/>
+      <c r="I459" s="12"/>
     </row>
     <row r="460" ht="20.35" customHeight="1">
       <c r="A460" s="15">
@@ -10830,6 +11491,7 @@
       <c r="F460" s="12"/>
       <c r="G460" s="12"/>
       <c r="H460" s="12"/>
+      <c r="I460" s="12"/>
     </row>
     <row r="461" ht="20.35" customHeight="1">
       <c r="A461" s="15">
@@ -10850,6 +11512,7 @@
       <c r="F461" s="12"/>
       <c r="G461" s="12"/>
       <c r="H461" s="12"/>
+      <c r="I461" s="12"/>
     </row>
     <row r="462" ht="20.35" customHeight="1">
       <c r="A462" s="10">
@@ -10870,6 +11533,7 @@
       <c r="F462" s="12"/>
       <c r="G462" s="12"/>
       <c r="H462" s="12"/>
+      <c r="I462" s="12"/>
     </row>
     <row r="463" ht="20.35" customHeight="1">
       <c r="A463" s="10">
@@ -10890,6 +11554,7 @@
       <c r="F463" s="12"/>
       <c r="G463" s="12"/>
       <c r="H463" s="12"/>
+      <c r="I463" s="12"/>
     </row>
     <row r="464" ht="20.35" customHeight="1">
       <c r="A464" s="10">
@@ -10910,6 +11575,7 @@
       <c r="F464" s="12"/>
       <c r="G464" s="12"/>
       <c r="H464" s="12"/>
+      <c r="I464" s="12"/>
     </row>
     <row r="465" ht="20.35" customHeight="1">
       <c r="A465" s="10">
@@ -10930,6 +11596,7 @@
       <c r="F465" s="12"/>
       <c r="G465" s="12"/>
       <c r="H465" s="12"/>
+      <c r="I465" s="12"/>
     </row>
     <row r="466" ht="20.35" customHeight="1">
       <c r="A466" s="10">
@@ -10950,6 +11617,7 @@
       <c r="F466" s="12"/>
       <c r="G466" s="12"/>
       <c r="H466" s="12"/>
+      <c r="I466" s="12"/>
     </row>
     <row r="467" ht="20.35" customHeight="1">
       <c r="A467" s="10">
@@ -10970,6 +11638,7 @@
       <c r="F467" s="12"/>
       <c r="G467" s="12"/>
       <c r="H467" s="12"/>
+      <c r="I467" s="12"/>
     </row>
     <row r="468" ht="20.35" customHeight="1">
       <c r="A468" s="10">
@@ -10990,6 +11659,7 @@
       <c r="F468" s="12"/>
       <c r="G468" s="12"/>
       <c r="H468" s="12"/>
+      <c r="I468" s="12"/>
     </row>
     <row r="469" ht="20.35" customHeight="1">
       <c r="A469" s="10">
@@ -11010,6 +11680,7 @@
       <c r="F469" s="12"/>
       <c r="G469" s="12"/>
       <c r="H469" s="12"/>
+      <c r="I469" s="12"/>
     </row>
     <row r="470" ht="20.35" customHeight="1">
       <c r="A470" s="10">
@@ -11030,6 +11701,7 @@
       <c r="F470" s="12"/>
       <c r="G470" s="12"/>
       <c r="H470" s="12"/>
+      <c r="I470" s="12"/>
     </row>
     <row r="471" ht="20.35" customHeight="1">
       <c r="A471" s="10">
@@ -11050,6 +11722,7 @@
       <c r="F471" s="12"/>
       <c r="G471" s="12"/>
       <c r="H471" s="12"/>
+      <c r="I471" s="12"/>
     </row>
     <row r="472" ht="20.35" customHeight="1">
       <c r="A472" s="15">
@@ -11070,6 +11743,7 @@
       <c r="F472" s="12"/>
       <c r="G472" s="12"/>
       <c r="H472" s="12"/>
+      <c r="I472" s="12"/>
     </row>
     <row r="473" ht="20.35" customHeight="1">
       <c r="A473" s="15">
@@ -11090,6 +11764,7 @@
       <c r="F473" s="12"/>
       <c r="G473" s="12"/>
       <c r="H473" s="12"/>
+      <c r="I473" s="12"/>
     </row>
     <row r="474" ht="20.35" customHeight="1">
       <c r="A474" s="15">
@@ -11110,6 +11785,7 @@
       <c r="F474" s="12"/>
       <c r="G474" s="12"/>
       <c r="H474" s="12"/>
+      <c r="I474" s="12"/>
     </row>
     <row r="475" ht="20.35" customHeight="1">
       <c r="A475" s="15">
@@ -11130,6 +11806,7 @@
       <c r="F475" s="12"/>
       <c r="G475" s="12"/>
       <c r="H475" s="12"/>
+      <c r="I475" s="12"/>
     </row>
     <row r="476" ht="20.35" customHeight="1">
       <c r="A476" s="15">
@@ -11150,6 +11827,7 @@
       <c r="F476" s="12"/>
       <c r="G476" s="12"/>
       <c r="H476" s="12"/>
+      <c r="I476" s="12"/>
     </row>
     <row r="477" ht="20.35" customHeight="1">
       <c r="A477" s="15">
@@ -11170,6 +11848,7 @@
       <c r="F477" s="12"/>
       <c r="G477" s="12"/>
       <c r="H477" s="12"/>
+      <c r="I477" s="12"/>
     </row>
     <row r="478" ht="20.35" customHeight="1">
       <c r="A478" s="15">
@@ -11190,6 +11869,7 @@
       <c r="F478" s="12"/>
       <c r="G478" s="12"/>
       <c r="H478" s="12"/>
+      <c r="I478" s="12"/>
     </row>
     <row r="479" ht="20.35" customHeight="1">
       <c r="A479" s="15">
@@ -11210,6 +11890,7 @@
       <c r="F479" s="12"/>
       <c r="G479" s="12"/>
       <c r="H479" s="12"/>
+      <c r="I479" s="12"/>
     </row>
     <row r="480" ht="20.35" customHeight="1">
       <c r="A480" s="15">
@@ -11230,6 +11911,7 @@
       <c r="F480" s="12"/>
       <c r="G480" s="12"/>
       <c r="H480" s="12"/>
+      <c r="I480" s="12"/>
     </row>
     <row r="481" ht="20.35" customHeight="1">
       <c r="A481" s="15">
@@ -11250,6 +11932,7 @@
       <c r="F481" s="12"/>
       <c r="G481" s="12"/>
       <c r="H481" s="12"/>
+      <c r="I481" s="12"/>
     </row>
     <row r="482" ht="20.35" customHeight="1">
       <c r="A482" s="10">
@@ -11270,6 +11953,7 @@
       <c r="F482" s="12"/>
       <c r="G482" s="12"/>
       <c r="H482" s="12"/>
+      <c r="I482" s="12"/>
     </row>
     <row r="483" ht="20.35" customHeight="1">
       <c r="A483" s="10">
@@ -11290,6 +11974,7 @@
       <c r="F483" s="12"/>
       <c r="G483" s="12"/>
       <c r="H483" s="12"/>
+      <c r="I483" s="12"/>
     </row>
     <row r="484" ht="20.35" customHeight="1">
       <c r="A484" s="10">
@@ -11310,6 +11995,7 @@
       <c r="F484" s="12"/>
       <c r="G484" s="12"/>
       <c r="H484" s="12"/>
+      <c r="I484" s="12"/>
     </row>
     <row r="485" ht="20.35" customHeight="1">
       <c r="A485" s="10">
@@ -11330,6 +12016,7 @@
       <c r="F485" s="12"/>
       <c r="G485" s="12"/>
       <c r="H485" s="12"/>
+      <c r="I485" s="12"/>
     </row>
     <row r="486" ht="20.35" customHeight="1">
       <c r="A486" s="10">
@@ -11350,6 +12037,7 @@
       <c r="F486" s="12"/>
       <c r="G486" s="12"/>
       <c r="H486" s="12"/>
+      <c r="I486" s="12"/>
     </row>
     <row r="487" ht="20.35" customHeight="1">
       <c r="A487" s="10">
@@ -11370,6 +12058,7 @@
       <c r="F487" s="12"/>
       <c r="G487" s="12"/>
       <c r="H487" s="12"/>
+      <c r="I487" s="12"/>
     </row>
     <row r="488" ht="20.35" customHeight="1">
       <c r="A488" s="10">
@@ -11390,6 +12079,7 @@
       <c r="F488" s="12"/>
       <c r="G488" s="12"/>
       <c r="H488" s="12"/>
+      <c r="I488" s="12"/>
     </row>
     <row r="489" ht="20.35" customHeight="1">
       <c r="A489" s="10">
@@ -11410,6 +12100,7 @@
       <c r="F489" s="12"/>
       <c r="G489" s="12"/>
       <c r="H489" s="12"/>
+      <c r="I489" s="12"/>
     </row>
     <row r="490" ht="20.35" customHeight="1">
       <c r="A490" s="10">
@@ -11430,6 +12121,7 @@
       <c r="F490" s="12"/>
       <c r="G490" s="12"/>
       <c r="H490" s="12"/>
+      <c r="I490" s="12"/>
     </row>
     <row r="491" ht="20.35" customHeight="1">
       <c r="A491" s="10">
@@ -11450,6 +12142,7 @@
       <c r="F491" s="12"/>
       <c r="G491" s="12"/>
       <c r="H491" s="12"/>
+      <c r="I491" s="12"/>
     </row>
     <row r="492" ht="20.35" customHeight="1">
       <c r="A492" s="15">
@@ -11470,6 +12163,7 @@
       <c r="F492" s="12"/>
       <c r="G492" s="12"/>
       <c r="H492" s="12"/>
+      <c r="I492" s="12"/>
     </row>
     <row r="493" ht="20.35" customHeight="1">
       <c r="A493" s="15">
@@ -11490,6 +12184,7 @@
       <c r="F493" s="12"/>
       <c r="G493" s="12"/>
       <c r="H493" s="12"/>
+      <c r="I493" s="12"/>
     </row>
     <row r="494" ht="20.35" customHeight="1">
       <c r="A494" s="15">
@@ -11510,6 +12205,7 @@
       <c r="F494" s="12"/>
       <c r="G494" s="12"/>
       <c r="H494" s="12"/>
+      <c r="I494" s="12"/>
     </row>
     <row r="495" ht="20.35" customHeight="1">
       <c r="A495" s="15">
@@ -11530,6 +12226,7 @@
       <c r="F495" s="12"/>
       <c r="G495" s="12"/>
       <c r="H495" s="12"/>
+      <c r="I495" s="12"/>
     </row>
     <row r="496" ht="20.35" customHeight="1">
       <c r="A496" s="15">
@@ -11550,6 +12247,7 @@
       <c r="F496" s="12"/>
       <c r="G496" s="12"/>
       <c r="H496" s="12"/>
+      <c r="I496" s="12"/>
     </row>
     <row r="497" ht="20.35" customHeight="1">
       <c r="A497" s="15">
@@ -11570,6 +12268,7 @@
       <c r="F497" s="12"/>
       <c r="G497" s="12"/>
       <c r="H497" s="12"/>
+      <c r="I497" s="12"/>
     </row>
     <row r="498" ht="20.35" customHeight="1">
       <c r="A498" s="15">
@@ -11590,6 +12289,7 @@
       <c r="F498" s="12"/>
       <c r="G498" s="12"/>
       <c r="H498" s="12"/>
+      <c r="I498" s="12"/>
     </row>
     <row r="499" ht="20.35" customHeight="1">
       <c r="A499" s="15">
@@ -11610,6 +12310,7 @@
       <c r="F499" s="12"/>
       <c r="G499" s="12"/>
       <c r="H499" s="12"/>
+      <c r="I499" s="12"/>
     </row>
     <row r="500" ht="20.35" customHeight="1">
       <c r="A500" s="15">
@@ -11630,6 +12331,7 @@
       <c r="F500" s="12"/>
       <c r="G500" s="12"/>
       <c r="H500" s="12"/>
+      <c r="I500" s="12"/>
     </row>
     <row r="501" ht="20.35" customHeight="1">
       <c r="A501" s="15">
@@ -11650,6 +12352,7 @@
       <c r="F501" s="12"/>
       <c r="G501" s="12"/>
       <c r="H501" s="12"/>
+      <c r="I501" s="12"/>
     </row>
     <row r="502" ht="20.35" customHeight="1">
       <c r="A502" s="10">
@@ -11670,6 +12373,7 @@
       <c r="F502" s="12"/>
       <c r="G502" s="12"/>
       <c r="H502" s="12"/>
+      <c r="I502" s="12"/>
     </row>
     <row r="503" ht="20.35" customHeight="1">
       <c r="A503" s="10">
@@ -11690,6 +12394,7 @@
       <c r="F503" s="12"/>
       <c r="G503" s="12"/>
       <c r="H503" s="12"/>
+      <c r="I503" s="12"/>
     </row>
     <row r="504" ht="20.35" customHeight="1">
       <c r="A504" s="10">
@@ -11710,6 +12415,7 @@
       <c r="F504" s="12"/>
       <c r="G504" s="12"/>
       <c r="H504" s="12"/>
+      <c r="I504" s="12"/>
     </row>
     <row r="505" ht="20.35" customHeight="1">
       <c r="A505" s="10">
@@ -11730,6 +12436,7 @@
       <c r="F505" s="12"/>
       <c r="G505" s="12"/>
       <c r="H505" s="12"/>
+      <c r="I505" s="12"/>
     </row>
     <row r="506" ht="20.35" customHeight="1">
       <c r="A506" s="10">
@@ -11750,6 +12457,7 @@
       <c r="F506" s="12"/>
       <c r="G506" s="12"/>
       <c r="H506" s="12"/>
+      <c r="I506" s="12"/>
     </row>
     <row r="507" ht="20.35" customHeight="1">
       <c r="A507" s="10">
@@ -11770,6 +12478,7 @@
       <c r="F507" s="12"/>
       <c r="G507" s="12"/>
       <c r="H507" s="12"/>
+      <c r="I507" s="12"/>
     </row>
     <row r="508" ht="20.35" customHeight="1">
       <c r="A508" s="10">
@@ -11790,6 +12499,7 @@
       <c r="F508" s="12"/>
       <c r="G508" s="12"/>
       <c r="H508" s="12"/>
+      <c r="I508" s="12"/>
     </row>
     <row r="509" ht="20.35" customHeight="1">
       <c r="A509" s="10">
@@ -11810,6 +12520,7 @@
       <c r="F509" s="12"/>
       <c r="G509" s="12"/>
       <c r="H509" s="12"/>
+      <c r="I509" s="12"/>
     </row>
     <row r="510" ht="20.35" customHeight="1">
       <c r="A510" s="10">
@@ -11830,6 +12541,7 @@
       <c r="F510" s="12"/>
       <c r="G510" s="12"/>
       <c r="H510" s="12"/>
+      <c r="I510" s="12"/>
     </row>
     <row r="511" ht="20.35" customHeight="1">
       <c r="A511" s="10">
@@ -11850,6 +12562,7 @@
       <c r="F511" s="12"/>
       <c r="G511" s="12"/>
       <c r="H511" s="12"/>
+      <c r="I511" s="12"/>
     </row>
     <row r="512" ht="20.35" customHeight="1">
       <c r="A512" s="15">
@@ -11870,6 +12583,7 @@
       <c r="F512" s="12"/>
       <c r="G512" s="12"/>
       <c r="H512" s="12"/>
+      <c r="I512" s="12"/>
     </row>
     <row r="513" ht="20.35" customHeight="1">
       <c r="A513" s="15">
@@ -11890,6 +12604,7 @@
       <c r="F513" s="12"/>
       <c r="G513" s="12"/>
       <c r="H513" s="12"/>
+      <c r="I513" s="12"/>
     </row>
     <row r="514" ht="20.35" customHeight="1">
       <c r="A514" s="15">
@@ -11910,6 +12625,7 @@
       <c r="F514" s="12"/>
       <c r="G514" s="12"/>
       <c r="H514" s="12"/>
+      <c r="I514" s="12"/>
     </row>
     <row r="515" ht="20.35" customHeight="1">
       <c r="A515" s="15">
@@ -11930,6 +12646,7 @@
       <c r="F515" s="12"/>
       <c r="G515" s="12"/>
       <c r="H515" s="12"/>
+      <c r="I515" s="12"/>
     </row>
     <row r="516" ht="20.35" customHeight="1">
       <c r="A516" s="15">
@@ -11950,6 +12667,7 @@
       <c r="F516" s="12"/>
       <c r="G516" s="12"/>
       <c r="H516" s="12"/>
+      <c r="I516" s="12"/>
     </row>
     <row r="517" ht="20.35" customHeight="1">
       <c r="A517" s="15">
@@ -11970,6 +12688,7 @@
       <c r="F517" s="12"/>
       <c r="G517" s="12"/>
       <c r="H517" s="12"/>
+      <c r="I517" s="12"/>
     </row>
     <row r="518" ht="20.35" customHeight="1">
       <c r="A518" s="15">
@@ -11990,6 +12709,7 @@
       <c r="F518" s="12"/>
       <c r="G518" s="12"/>
       <c r="H518" s="12"/>
+      <c r="I518" s="12"/>
     </row>
     <row r="519" ht="20.35" customHeight="1">
       <c r="A519" s="15">
@@ -12010,6 +12730,7 @@
       <c r="F519" s="12"/>
       <c r="G519" s="12"/>
       <c r="H519" s="12"/>
+      <c r="I519" s="12"/>
     </row>
     <row r="520" ht="20.35" customHeight="1">
       <c r="A520" s="15">
@@ -12030,6 +12751,7 @@
       <c r="F520" s="12"/>
       <c r="G520" s="12"/>
       <c r="H520" s="12"/>
+      <c r="I520" s="12"/>
     </row>
     <row r="521" ht="20.35" customHeight="1">
       <c r="A521" s="15">
@@ -12050,6 +12772,7 @@
       <c r="F521" s="12"/>
       <c r="G521" s="12"/>
       <c r="H521" s="12"/>
+      <c r="I521" s="12"/>
     </row>
     <row r="522" ht="20.35" customHeight="1">
       <c r="A522" s="10">
@@ -12070,6 +12793,7 @@
       <c r="F522" s="12"/>
       <c r="G522" s="12"/>
       <c r="H522" s="12"/>
+      <c r="I522" s="12"/>
     </row>
     <row r="523" ht="20.35" customHeight="1">
       <c r="A523" s="10">
@@ -12090,6 +12814,7 @@
       <c r="F523" s="12"/>
       <c r="G523" s="12"/>
       <c r="H523" s="12"/>
+      <c r="I523" s="12"/>
     </row>
     <row r="524" ht="20.35" customHeight="1">
       <c r="A524" s="10">
@@ -12110,6 +12835,7 @@
       <c r="F524" s="12"/>
       <c r="G524" s="12"/>
       <c r="H524" s="12"/>
+      <c r="I524" s="12"/>
     </row>
     <row r="525" ht="20.35" customHeight="1">
       <c r="A525" s="10">
@@ -12130,6 +12856,7 @@
       <c r="F525" s="12"/>
       <c r="G525" s="12"/>
       <c r="H525" s="12"/>
+      <c r="I525" s="12"/>
     </row>
     <row r="526" ht="20.35" customHeight="1">
       <c r="A526" s="10">
@@ -12150,6 +12877,7 @@
       <c r="F526" s="12"/>
       <c r="G526" s="12"/>
       <c r="H526" s="12"/>
+      <c r="I526" s="12"/>
     </row>
     <row r="527" ht="20.35" customHeight="1">
       <c r="A527" s="10">
@@ -12170,6 +12898,7 @@
       <c r="F527" s="12"/>
       <c r="G527" s="12"/>
       <c r="H527" s="12"/>
+      <c r="I527" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>